<commit_message>
Clean services data and export as .csv
</commit_message>
<xml_diff>
--- a/backend/api/servicehandler/services/ABA IBI Providers.xlsx
+++ b/backend/api/servicehandler/services/ABA IBI Providers.xlsx
@@ -1,27 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://utoronto-my.sharepoint.com/personal/behnaz_merikhi_utoronto_ca/Documents/ASD Project/DB/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dextertam/Documents/UofT/Y3/_Extracurricular/AutismCanadaAI/backend/api/servicehandler/services/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{3F7D9D29-FF0B-46FB-975F-D4C7ADA165B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{343F658E-99B6-7545-AAA9-2A6C7CCB7BD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="-28300" windowWidth="51200" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Recovered_Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="756" uniqueCount="690">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="755" uniqueCount="684">
   <si>
     <t>https://www.myautismguide.ca/mag/content/provider/1-step-ahead-services-inc?nid=561321</t>
   </si>
@@ -56,9 +55,6 @@
     <t>ON</t>
   </si>
   <si>
-    <t>519-257-8259</t>
-  </si>
-  <si>
     <t>https://www.myautismguide.ca/mag/content/provider/block-above-behavioral-consulting?nid=561331</t>
   </si>
   <si>
@@ -236,9 +232,6 @@
     <t>335 Habkirk Dr Regina, SKS4S 6A9</t>
   </si>
   <si>
-    <t>306-570-4273</t>
-  </si>
-  <si>
     <t>https://www.myautismguide.ca/mag/content/provider/above-and-beyond-autism-consulting-services?nid=581146</t>
   </si>
   <si>
@@ -293,9 +286,6 @@
     <t>36 antares Drive Ottawa, ONK2E 7W5</t>
   </si>
   <si>
-    <t>343-887-2287</t>
-  </si>
-  <si>
     <t>https://www.myautismguide.ca/mag/content/provider/aim-pediatric-therapy-2?nid=569731</t>
   </si>
   <si>
@@ -377,9 +367,6 @@
     <t>36-5200 Dallas Drive Kamloops, BCV2C 6Y8</t>
   </si>
   <si>
-    <t>250-299-3530</t>
-  </si>
-  <si>
     <t>https://www.myautismguide.ca/mag/content/provider/applied-behavioural-interventions?nid=569861</t>
   </si>
   <si>
@@ -437,9 +424,6 @@
     <t>2006 Robertson rd Ottawa, ON</t>
   </si>
   <si>
-    <t>(613) 680-4700          (613) 424-0442</t>
-  </si>
-  <si>
     <t>https://www.myautismguide.ca/mag/content/provider/aspiration-discoveries?nid=569916</t>
   </si>
   <si>
@@ -776,9 +760,6 @@
     <t>L3 30 Dupont Street East Waterloo, ONN2J 2G9</t>
   </si>
   <si>
-    <t>226-755-0015</t>
-  </si>
-  <si>
     <t>https://www.myautismguide.ca/mag/content/provider/beyond-services-choice-matters?nid=570386</t>
   </si>
   <si>
@@ -812,9 +793,6 @@
     <t>5836 Leslie Street Suite 809 Toronto, ONM2H 1J8</t>
   </si>
   <si>
-    <t>416-554-8716</t>
-  </si>
-  <si>
     <t>https://www.myautismguide.ca/mag/content/provider/beyond-spectrum?nid=570396</t>
   </si>
   <si>
@@ -872,9 +850,6 @@
     <t>85 Le Maire St. Winnipeg, MBR3V 1E1</t>
   </si>
   <si>
-    <t>431-531-8701</t>
-  </si>
-  <si>
     <t>https://www.myautismguide.ca/mag/content/provider/blue-lantern-learning?nid=566766</t>
   </si>
   <si>
@@ -1094,9 +1069,6 @@
     <t>3rd Floor, WMRH P.O Box 2005 Corner Brooke, NLA2H 6J7</t>
   </si>
   <si>
-    <t>7096375000 6655</t>
-  </si>
-  <si>
     <t>https://www.myautismguide.ca/mag/content/provider/childrens-development-group?nid=571431</t>
   </si>
   <si>
@@ -1202,9 +1174,6 @@
     <t>Markham, ON</t>
   </si>
   <si>
-    <t>416-993-4369</t>
-  </si>
-  <si>
     <t>https://www.myautismguide.ca/mag/content/provider/dr-kiran-pure-associates?nid=568496</t>
   </si>
   <si>
@@ -1307,9 +1276,6 @@
     <t>10145 McVean Drive   Brampton,, ONL6P 4K7</t>
   </si>
   <si>
-    <t>1-877-374-6625</t>
-  </si>
-  <si>
     <t>https://www.myautismguide.ca/mag/content/provider/erinoakkids-centre-treatment-and-development-0?nid=585846</t>
   </si>
   <si>
@@ -1337,9 +1303,6 @@
     <t>520 Westney Road S Ajax, ONL1S 6W4</t>
   </si>
   <si>
-    <t>1(866) 211-7779</t>
-  </si>
-  <si>
     <t>https://www.myautismguide.ca/mag/content/provider/exceptional-minds?nid=572641</t>
   </si>
   <si>
@@ -1385,9 +1348,6 @@
     <t>5703, rue Ferrier Mont-Royal, QCH4P 1N3</t>
   </si>
   <si>
-    <t>514.345.1300</t>
-  </si>
-  <si>
     <t>https://www.myautismguide.ca/mag/content/provider/functional-learning-centre?nid=563176</t>
   </si>
   <si>
@@ -1511,9 +1471,6 @@
     <t>14487 78th Avenue  Surrey, BCV3S 9C5</t>
   </si>
   <si>
-    <t>604-572-1126</t>
-  </si>
-  <si>
     <t>https://www.myautismguide.ca/mag/content/provider/helping-hands-behaviour-consulting?nid=563381</t>
   </si>
   <si>
@@ -1556,9 +1513,6 @@
     <t>231 Elm Beaconsfield, QCH9W 2E2</t>
   </si>
   <si>
-    <t>5146953914#3304</t>
-  </si>
-  <si>
     <t>https://www.myautismguide.ca/mag/content/provider/i-believe-miracles?nid=573331</t>
   </si>
   <si>
@@ -1643,9 +1597,6 @@
     <t>Durham Region, ON</t>
   </si>
   <si>
-    <t>905-914-0405</t>
-  </si>
-  <si>
     <t>https://www.myautismguide.ca/mag/content/provider/jhmj-coaching-consulting?nid=562846</t>
   </si>
   <si>
@@ -1655,9 +1606,6 @@
     <t>BC</t>
   </si>
   <si>
-    <t>250-597-8997</t>
-  </si>
-  <si>
     <t>https://www.myautismguide.ca/mag/content/provider/joy-behaviour-consulting-intervention?nid=559841</t>
   </si>
   <si>
@@ -1697,9 +1645,6 @@
     <t>Ottawa, ON</t>
   </si>
   <si>
-    <t>613-327-5775</t>
-  </si>
-  <si>
     <t>https://www.myautismguide.ca/mag/content/provider/mcmaster-autism-program?nid=601316</t>
   </si>
   <si>
@@ -1709,9 +1654,6 @@
     <t>325 Wellington St N Hamilton , ONM5V 1E7</t>
   </si>
   <si>
-    <t>905-521-2100</t>
-  </si>
-  <si>
     <t>https://www.myautismguide.ca/mag/content/provider/moving-forward-autism-services-tools-inc?nid=588541</t>
   </si>
   <si>
@@ -1721,9 +1663,6 @@
     <t>1200 Lawrence Ave East Suite 304 North York, ONM3A 1C1</t>
   </si>
   <si>
-    <t>647-468-0474</t>
-  </si>
-  <si>
     <t>https://www.myautismguide.ca/mag/content/provider/nunavummi-disabilities-makinnasuaqtiit-society?nid=588576</t>
   </si>
   <si>
@@ -1733,9 +1672,6 @@
     <t>PO Box 4212 Iqaluit, NUX0A1H0</t>
   </si>
   <si>
-    <t>867-979-2228</t>
-  </si>
-  <si>
     <t>https://www.myautismguide.ca/mag/content/provider/oap-provider-list?nid=593141</t>
   </si>
   <si>
@@ -1751,18 +1687,12 @@
     <t>32 Elgin St. East Oshawa, ONL1G1T1</t>
   </si>
   <si>
-    <t>4164549340</t>
-  </si>
-  <si>
     <t>https://www.myautismguide.ca/mag/content/provider/one-care-inc-0?nid=588586</t>
   </si>
   <si>
     <t>169-173 Simcoe St. North Oshawa, ONL1G 4S8</t>
   </si>
   <si>
-    <t>905 2402203</t>
-  </si>
-  <si>
     <t>https://www.myautismguide.ca/mag/content/provider/osns-child-youth-development-centre?nid=564966</t>
   </si>
   <si>
@@ -1784,9 +1714,6 @@
     <t>12-52 Antares Ottawa, ONK2E 7Z1</t>
   </si>
   <si>
-    <t>(613)212-4828</t>
-  </si>
-  <si>
     <t>https://www.myautismguide.ca/mag/content/provider/parley-services-limited?nid=588611</t>
   </si>
   <si>
@@ -1796,9 +1723,6 @@
     <t>Suite 1703, 805 West Broadway Vancouver, BCV5Z 1K1</t>
   </si>
   <si>
-    <t>604-868-5586</t>
-  </si>
-  <si>
     <t>https://www.myautismguide.ca/mag/content/provider/pivot-point-family-growth-centre-inc-11?nid=588626</t>
   </si>
   <si>
@@ -1808,9 +1732,6 @@
     <t>#24 15515 24th Avenue Surrey, BCV4A 2J4</t>
   </si>
   <si>
-    <t>604.531.4544</t>
-  </si>
-  <si>
     <t>https://www.myautismguide.ca/mag/content/provider/positive-behavioral-supports-corp-canada?nid=588631</t>
   </si>
   <si>
@@ -1820,9 +1741,6 @@
     <t>99 Oswell Dr. Ajax, ONL1Z 0L5</t>
   </si>
   <si>
-    <t>6473602700 X 1163</t>
-  </si>
-  <si>
     <t>https://www.myautismguide.ca/mag/content/provider/precious-souls-services-inc?nid=588636</t>
   </si>
   <si>
@@ -1832,18 +1750,12 @@
     <t>7330 Goreway Drive Mississauga, ONL4T 4J2</t>
   </si>
   <si>
-    <t>647-948-8080</t>
-  </si>
-  <si>
     <t>https://www.myautismguide.ca/mag/content/provider/santana-behavioural-services?nid=588681</t>
   </si>
   <si>
     <t>Santana Behavioural Services</t>
   </si>
   <si>
-    <t>647-588-0271</t>
-  </si>
-  <si>
     <t>https://www.myautismguide.ca/mag/content/provider/shining-through-centre-2?nid=588701</t>
   </si>
   <si>
@@ -1853,9 +1765,6 @@
     <t>7365 Martin Grove Rd Woodbridge, ONL4L 9E4</t>
   </si>
   <si>
-    <t>905-851-7955</t>
-  </si>
-  <si>
     <t>https://www.myautismguide.ca/mag/content/provider/south-asian-autism-awareness-center?nid=577136</t>
   </si>
   <si>
@@ -1877,9 +1786,6 @@
     <t>489c Tennyson Place Victoria, BCV8Z 3P6</t>
   </si>
   <si>
-    <t>250-472-8304</t>
-  </si>
-  <si>
     <t>https://www.myautismguide.ca/mag/content/provider/success-steps-0?nid=588766</t>
   </si>
   <si>
@@ -1889,9 +1795,6 @@
     <t>13 Dallas Place Ottawa, ONK2G 3E2</t>
   </si>
   <si>
-    <t>613-882-7688</t>
-  </si>
-  <si>
     <t>https://www.myautismguide.ca/mag/content/provider/sue-larke?nid=560121</t>
   </si>
   <si>
@@ -1925,9 +1828,6 @@
     <t>547 Upper James Street Hamilton, ONL9C 2Y5</t>
   </si>
   <si>
-    <t>289-755-7891</t>
-  </si>
-  <si>
     <t>https://www.myautismguide.ca/mag/content/provider/teach-me-my-way-services-0?nid=597546</t>
   </si>
   <si>
@@ -1943,9 +1843,6 @@
     <t>685 Kennedy Road #5 Scarborough , ONM1K 2B8</t>
   </si>
   <si>
-    <t>647-330-6130</t>
-  </si>
-  <si>
     <t>https://www.myautismguide.ca/mag/content/provider/birch-centre-learning-and-development-aba-therapy?nid=595071</t>
   </si>
   <si>
@@ -1967,9 +1864,6 @@
     <t>63 Fernbank Place  Whitby, ONL1R 1T1</t>
   </si>
   <si>
-    <t>905 626 0377</t>
-  </si>
-  <si>
     <t>https://www.myautismguide.ca/mag/content/provider/toronto-ibi-0?nid=588811</t>
   </si>
   <si>
@@ -1979,9 +1873,6 @@
     <t>32-1170 Sheppard Ave. W North York, ONM3K 2A3</t>
   </si>
   <si>
-    <t>416-614-9025</t>
-  </si>
-  <si>
     <t>https://www.myautismguide.ca/mag/content/provider/toronto-ibi-1?nid=588816</t>
   </si>
   <si>
@@ -1997,9 +1888,6 @@
     <t>Suite 112/210 2800 High Point Drive Milton, ONL9T 6P4</t>
   </si>
   <si>
-    <t>365 877 9094</t>
-  </si>
-  <si>
     <t>https://www.myautismguide.ca/mag/content/provider/valley-child-development-association-0?nid=588841</t>
   </si>
   <si>
@@ -2009,9 +1897,6 @@
     <t>28 Aberdeen St, Suite 5 Kentville, NSB4N 2N1</t>
   </si>
   <si>
-    <t>902-678-6111</t>
-  </si>
-  <si>
     <t>https://www.myautismguide.ca/mag/content/provider/wes-consortium?nid=589301</t>
   </si>
   <si>
@@ -2021,9 +1906,6 @@
     <t>Brampton, ON</t>
   </si>
   <si>
-    <t>905-439-9280</t>
-  </si>
-  <si>
     <t>https://www.myautismguide.ca/mag/content/provider/wirth-behavioural-health-services?nid=567201</t>
   </si>
   <si>
@@ -2042,9 +1924,6 @@
     <t>32 Woodstone Dr East St. Paul, MBR2E 0M5</t>
   </si>
   <si>
-    <t>204-807-6779</t>
-  </si>
-  <si>
     <t>https://www.myautismguide.ca/mag/content/provider/woodview-mental-health-autism-services?nid=578426</t>
   </si>
   <si>
@@ -2054,9 +1933,6 @@
     <t>50 Fairwood Place W Burlington, ONL7T 1E5</t>
   </si>
   <si>
-    <t>905 689 4727</t>
-  </si>
-  <si>
     <t>https://www.myautismguide.ca/mag/content/provider/woodview-mental-health-and-autism-services?nid=578486</t>
   </si>
   <si>
@@ -2066,9 +1942,6 @@
     <t>643 Park Road North Brantford, ONN3T 5L8</t>
   </si>
   <si>
-    <t>519 752 5308</t>
-  </si>
-  <si>
     <t>https://www.myautismguide.ca/mag/content/provider/york-autism-centre-making-small-talk?nid=588901</t>
   </si>
   <si>
@@ -2078,9 +1951,6 @@
     <t>73 Industrial Parkway North - Unit 4 Aurora, ONL4C 4C4</t>
   </si>
   <si>
-    <t>647-519-6739</t>
-  </si>
-  <si>
     <t>Organization</t>
   </si>
   <si>
@@ -2091,13 +1961,124 @@
   </si>
   <si>
     <t>Phone</t>
+  </si>
+  <si>
+    <t>(519) 257-8259</t>
+  </si>
+  <si>
+    <t>(343) 887-2287</t>
+  </si>
+  <si>
+    <t>(431) 531-8701</t>
+  </si>
+  <si>
+    <t>(877) 374-6625</t>
+  </si>
+  <si>
+    <t>(866) 211-7779</t>
+  </si>
+  <si>
+    <t>(514) 345-1300</t>
+  </si>
+  <si>
+    <t>(905) 914-0405</t>
+  </si>
+  <si>
+    <t>(250) 597-8997</t>
+  </si>
+  <si>
+    <t>(613) 327-5775</t>
+  </si>
+  <si>
+    <t>(905) 521-2100</t>
+  </si>
+  <si>
+    <t>(647) 468-0474</t>
+  </si>
+  <si>
+    <t>(867) 979-2228</t>
+  </si>
+  <si>
+    <t>(416) 454-9340</t>
+  </si>
+  <si>
+    <t>(905) 240-2203</t>
+  </si>
+  <si>
+    <t>(604) 868-5586</t>
+  </si>
+  <si>
+    <t>(604) 531-4544</t>
+  </si>
+  <si>
+    <t>(647) 948-8080</t>
+  </si>
+  <si>
+    <t>(647) 588-0271</t>
+  </si>
+  <si>
+    <t>(905) 851-7955</t>
+  </si>
+  <si>
+    <t>(250) 472-8304</t>
+  </si>
+  <si>
+    <t>(613) 882-7688</t>
+  </si>
+  <si>
+    <t>(289) 755-7891</t>
+  </si>
+  <si>
+    <t>(289) 755-7892</t>
+  </si>
+  <si>
+    <t>(647) 330-6130</t>
+  </si>
+  <si>
+    <t>(905) 626-0377</t>
+  </si>
+  <si>
+    <t>(416) 614-9025</t>
+  </si>
+  <si>
+    <t>(365) 877-9094</t>
+  </si>
+  <si>
+    <t>(902) 678-6111</t>
+  </si>
+  <si>
+    <t>(905) 439-9280</t>
+  </si>
+  <si>
+    <t>(204) 807-6780</t>
+  </si>
+  <si>
+    <t>(905) 689-4727</t>
+  </si>
+  <si>
+    <t>(519) 752-5308</t>
+  </si>
+  <si>
+    <t>(647) 519-6739</t>
+  </si>
+  <si>
+    <t>(613) 680-4700</t>
+  </si>
+  <si>
+    <t>(613) 212-4828</t>
+  </si>
+  <si>
+    <t>(514) 695-3914</t>
+  </si>
+  <si>
+    <t>(709) 637-5000 6655</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2109,6 +2090,12 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -2478,33 +2465,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D189"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+    <sheetView tabSelected="1" zoomScale="132" workbookViewId="0">
+      <selection activeCell="F92" sqref="F92"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="53.625" customWidth="1"/>
-    <col min="2" max="2" width="35.25" customWidth="1"/>
-    <col min="3" max="3" width="39.875" customWidth="1"/>
-    <col min="4" max="4" width="31.625" customWidth="1"/>
+    <col min="1" max="1" width="93" customWidth="1"/>
+    <col min="2" max="2" width="60.6640625" customWidth="1"/>
+    <col min="3" max="3" width="35.33203125" customWidth="1"/>
+    <col min="4" max="4" width="31.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>687</v>
+        <v>644</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>686</v>
+        <v>643</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>688</v>
+        <v>645</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>689</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2518,7 +2505,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -2532,7 +2519,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -2543,2600 +2530,2598 @@
         <v>10</v>
       </c>
       <c r="D4" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="B5" t="s">
         <v>12</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>13</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>14</v>
       </c>
-      <c r="D5" t="s">
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="B6" t="s">
         <v>16</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>17</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>18</v>
       </c>
-      <c r="D6" t="s">
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="B7" t="s">
         <v>20</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>21</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>22</v>
       </c>
-      <c r="D7" t="s">
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="B8" t="s">
         <v>24</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>25</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>26</v>
       </c>
-      <c r="D8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="B9" t="s">
         <v>27</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>28</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>29</v>
       </c>
-      <c r="D9" t="s">
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="B10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" t="s">
         <v>31</v>
       </c>
-      <c r="B10" t="s">
-        <v>28</v>
-      </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>32</v>
       </c>
-      <c r="D10" t="s">
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="B11" t="s">
         <v>34</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>35</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>36</v>
       </c>
-      <c r="D11" t="s">
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="B12" t="s">
         <v>38</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>39</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>40</v>
       </c>
-      <c r="D12" t="s">
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="B13" t="s">
         <v>42</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>43</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>44</v>
       </c>
-      <c r="D13" t="s">
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="B14" t="s">
         <v>46</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>47</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>48</v>
       </c>
-      <c r="D14" t="s">
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="B15" t="s">
         <v>50</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>51</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>52</v>
       </c>
-      <c r="D15" t="s">
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="B16" t="s">
         <v>54</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>55</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>56</v>
       </c>
-      <c r="D16" t="s">
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="B17" t="s">
         <v>58</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>59</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>60</v>
       </c>
-      <c r="D17" t="s">
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="B18" t="s">
+        <v>58</v>
+      </c>
+      <c r="C18" t="s">
         <v>62</v>
       </c>
-      <c r="B18" t="s">
-        <v>59</v>
-      </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>63</v>
       </c>
-      <c r="D18" t="s">
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="B19" t="s">
+        <v>58</v>
+      </c>
+      <c r="C19" t="s">
         <v>65</v>
       </c>
-      <c r="B19" t="s">
-        <v>59</v>
-      </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>66</v>
       </c>
-      <c r="D19" t="s">
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="B20" t="s">
         <v>68</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>69</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
         <v>70</v>
       </c>
-      <c r="D20" t="s">
+      <c r="B21" t="s">
+        <v>68</v>
+      </c>
+      <c r="C21" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="D21" t="s">
         <v>72</v>
       </c>
-      <c r="B21" t="s">
-        <v>69</v>
-      </c>
-      <c r="C21" t="s">
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
         <v>73</v>
       </c>
-      <c r="D21" t="s">
+      <c r="B22" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="C22" t="s">
         <v>75</v>
       </c>
-      <c r="B22" t="s">
+      <c r="D22" t="s">
         <v>76</v>
       </c>
-      <c r="C22" t="s">
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
         <v>77</v>
       </c>
-      <c r="D22" t="s">
+      <c r="B23" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="C23" t="s">
         <v>79</v>
       </c>
-      <c r="B23" t="s">
+      <c r="D23" t="s">
         <v>80</v>
       </c>
-      <c r="C23" t="s">
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
         <v>81</v>
       </c>
-      <c r="D23" t="s">
+      <c r="B24" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="C24" t="s">
         <v>83</v>
       </c>
-      <c r="B24" t="s">
+      <c r="D24" t="s">
         <v>84</v>
       </c>
-      <c r="C24" t="s">
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
         <v>85</v>
       </c>
-      <c r="D24" t="s">
+      <c r="B25" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="C25" t="s">
         <v>87</v>
       </c>
-      <c r="B25" t="s">
+      <c r="D25" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
         <v>88</v>
       </c>
-      <c r="C25" t="s">
+      <c r="B26" t="s">
         <v>89</v>
       </c>
-      <c r="D25" t="s">
+      <c r="C26" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="D26" t="s">
         <v>91</v>
       </c>
-      <c r="B26" t="s">
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
         <v>92</v>
       </c>
-      <c r="C26" t="s">
+      <c r="B27" t="s">
+        <v>89</v>
+      </c>
+      <c r="C27" t="s">
         <v>93</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D27" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="B28" t="s">
+        <v>89</v>
+      </c>
+      <c r="C28" t="s">
         <v>95</v>
       </c>
-      <c r="B27" t="s">
-        <v>92</v>
-      </c>
-      <c r="C27" t="s">
+      <c r="D28" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
         <v>96</v>
       </c>
-      <c r="D27" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="B29" t="s">
+        <v>89</v>
+      </c>
+      <c r="C29" t="s">
         <v>97</v>
       </c>
-      <c r="B28" t="s">
-        <v>92</v>
-      </c>
-      <c r="C28" t="s">
+      <c r="D29" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
         <v>98</v>
       </c>
-      <c r="D28" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="B30" t="s">
+        <v>89</v>
+      </c>
+      <c r="C30" t="s">
         <v>99</v>
       </c>
-      <c r="B29" t="s">
-        <v>92</v>
-      </c>
-      <c r="C29" t="s">
+      <c r="D30" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
         <v>100</v>
       </c>
-      <c r="D29" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+      <c r="B31" t="s">
+        <v>89</v>
+      </c>
+      <c r="C31" t="s">
         <v>101</v>
       </c>
-      <c r="B30" t="s">
-        <v>92</v>
-      </c>
-      <c r="C30" t="s">
+      <c r="D31" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
         <v>102</v>
       </c>
-      <c r="D30" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+      <c r="B32" t="s">
+        <v>89</v>
+      </c>
+      <c r="C32" t="s">
         <v>103</v>
       </c>
-      <c r="B31" t="s">
-        <v>92</v>
-      </c>
-      <c r="C31" t="s">
+      <c r="D32" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
         <v>104</v>
       </c>
-      <c r="D31" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+      <c r="B33" t="s">
         <v>105</v>
       </c>
-      <c r="B32" t="s">
-        <v>92</v>
-      </c>
-      <c r="C32" t="s">
+      <c r="C33" t="s">
         <v>106</v>
       </c>
-      <c r="D32" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+      <c r="D33" t="s">
         <v>107</v>
       </c>
-      <c r="B33" t="s">
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
         <v>108</v>
       </c>
-      <c r="C33" t="s">
+      <c r="B34" t="s">
         <v>109</v>
       </c>
-      <c r="D33" t="s">
+      <c r="C34" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+      <c r="D34" t="s">
         <v>111</v>
       </c>
-      <c r="B34" t="s">
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
         <v>112</v>
       </c>
-      <c r="C34" t="s">
+      <c r="B35" t="s">
         <v>113</v>
       </c>
-      <c r="D34" t="s">
+      <c r="C35" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+      <c r="D35" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
         <v>115</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B36" t="s">
         <v>116</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C36" t="s">
         <v>117</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D36" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
         <v>119</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B37" t="s">
         <v>120</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C37" t="s">
         <v>121</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D37" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
         <v>123</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B38" t="s">
         <v>124</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C38" t="s">
         <v>125</v>
       </c>
-      <c r="D37" t="s">
+      <c r="D38" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
         <v>127</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B39" t="s">
         <v>128</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C39" t="s">
         <v>129</v>
       </c>
-      <c r="D38" t="s">
+      <c r="D39" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
         <v>131</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B40" t="s">
         <v>132</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C40" t="s">
         <v>133</v>
       </c>
-      <c r="D39" t="s">
+      <c r="D40" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+      <c r="B41" t="s">
         <v>135</v>
       </c>
-      <c r="B40" t="s">
+      <c r="C41" t="s">
         <v>136</v>
       </c>
-      <c r="C40" t="s">
+      <c r="D41" t="s">
         <v>137</v>
       </c>
-      <c r="D40" t="s">
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+      <c r="B42" t="s">
         <v>139</v>
       </c>
-      <c r="B41" t="s">
+      <c r="C42" t="s">
         <v>140</v>
       </c>
-      <c r="C41" t="s">
+      <c r="D42" t="s">
         <v>141</v>
       </c>
-      <c r="D41" t="s">
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+      <c r="B43" t="s">
         <v>143</v>
       </c>
-      <c r="B42" t="s">
+      <c r="C43" t="s">
         <v>144</v>
       </c>
-      <c r="C42" t="s">
+      <c r="D43" t="s">
         <v>145</v>
       </c>
-      <c r="D42" t="s">
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+      <c r="B44" t="s">
         <v>147</v>
       </c>
-      <c r="B43" t="s">
+      <c r="C44" t="s">
         <v>148</v>
       </c>
-      <c r="C43" t="s">
+      <c r="D44" t="s">
         <v>149</v>
       </c>
-      <c r="D43" t="s">
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+      <c r="B45" t="s">
         <v>151</v>
       </c>
-      <c r="B44" t="s">
+      <c r="C45" t="s">
         <v>152</v>
       </c>
-      <c r="C44" t="s">
+      <c r="D45" t="s">
         <v>153</v>
       </c>
-      <c r="D44" t="s">
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+      <c r="B46" t="s">
         <v>155</v>
       </c>
-      <c r="B45" t="s">
+      <c r="C46" t="s">
         <v>156</v>
       </c>
-      <c r="C45" t="s">
+      <c r="D46" t="s">
         <v>157</v>
       </c>
-      <c r="D45" t="s">
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+      <c r="B47" t="s">
         <v>159</v>
       </c>
-      <c r="B46" t="s">
+      <c r="C47" t="s">
         <v>160</v>
       </c>
-      <c r="C46" t="s">
+      <c r="D47" t="s">
         <v>161</v>
       </c>
-      <c r="D46" t="s">
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+      <c r="B48" t="s">
         <v>163</v>
       </c>
-      <c r="B47" t="s">
+      <c r="C48" t="s">
         <v>164</v>
       </c>
-      <c r="C47" t="s">
+      <c r="D48" t="s">
         <v>165</v>
       </c>
-      <c r="D47" t="s">
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
+      <c r="B49" t="s">
         <v>167</v>
       </c>
-      <c r="B48" t="s">
+      <c r="C49" t="s">
         <v>168</v>
       </c>
-      <c r="C48" t="s">
+      <c r="D49" t="s">
         <v>169</v>
       </c>
-      <c r="D48" t="s">
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
+      <c r="B50" t="s">
+        <v>167</v>
+      </c>
+      <c r="C50" t="s">
         <v>171</v>
       </c>
-      <c r="B49" t="s">
+      <c r="D50" t="s">
         <v>172</v>
       </c>
-      <c r="C49" t="s">
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
         <v>173</v>
       </c>
-      <c r="D49" t="s">
+      <c r="B51" t="s">
+        <v>167</v>
+      </c>
+      <c r="C51" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
+      <c r="D51" t="s">
         <v>175</v>
       </c>
-      <c r="B50" t="s">
-        <v>172</v>
-      </c>
-      <c r="C50" t="s">
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
         <v>176</v>
       </c>
-      <c r="D50" t="s">
+      <c r="B52" t="s">
+        <v>167</v>
+      </c>
+      <c r="C52" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
+      <c r="D52" t="s">
         <v>178</v>
       </c>
-      <c r="B51" t="s">
-        <v>172</v>
-      </c>
-      <c r="C51" t="s">
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
         <v>179</v>
       </c>
-      <c r="D51" t="s">
+      <c r="B53" t="s">
+        <v>167</v>
+      </c>
+      <c r="C53" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
+      <c r="D53" t="s">
         <v>181</v>
       </c>
-      <c r="B52" t="s">
-        <v>172</v>
-      </c>
-      <c r="C52" t="s">
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
         <v>182</v>
       </c>
-      <c r="D52" t="s">
+      <c r="B54" t="s">
+        <v>167</v>
+      </c>
+      <c r="C54" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
+      <c r="D54" t="s">
         <v>184</v>
       </c>
-      <c r="B53" t="s">
-        <v>172</v>
-      </c>
-      <c r="C53" t="s">
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
         <v>185</v>
       </c>
-      <c r="D53" t="s">
+      <c r="B55" t="s">
+        <v>167</v>
+      </c>
+      <c r="C55" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
+      <c r="D55" t="s">
         <v>187</v>
       </c>
-      <c r="B54" t="s">
-        <v>172</v>
-      </c>
-      <c r="C54" t="s">
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
         <v>188</v>
       </c>
-      <c r="D54" t="s">
+      <c r="B56" t="s">
+        <v>167</v>
+      </c>
+      <c r="C56" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
+      <c r="D56" t="s">
         <v>190</v>
       </c>
-      <c r="B55" t="s">
-        <v>172</v>
-      </c>
-      <c r="C55" t="s">
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
         <v>191</v>
       </c>
-      <c r="D55" t="s">
+      <c r="B57" t="s">
+        <v>167</v>
+      </c>
+      <c r="C57" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
+      <c r="D57" t="s">
         <v>193</v>
       </c>
-      <c r="B56" t="s">
-        <v>172</v>
-      </c>
-      <c r="C56" t="s">
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
         <v>194</v>
       </c>
-      <c r="D56" t="s">
+      <c r="B58" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
+      <c r="C58" t="s">
         <v>196</v>
       </c>
-      <c r="B57" t="s">
-        <v>172</v>
-      </c>
-      <c r="C57" t="s">
+      <c r="D58" t="s">
         <v>197</v>
       </c>
-      <c r="D57" t="s">
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
+      <c r="B59" t="s">
         <v>199</v>
       </c>
-      <c r="B58" t="s">
+      <c r="C59" t="s">
         <v>200</v>
       </c>
-      <c r="C58" t="s">
+      <c r="D59" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
         <v>201</v>
       </c>
-      <c r="D58" t="s">
+      <c r="B60" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
+      <c r="C60" t="s">
         <v>203</v>
       </c>
-      <c r="B59" t="s">
+      <c r="D60" t="s">
         <v>204</v>
       </c>
-      <c r="C59" t="s">
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
         <v>205</v>
       </c>
-      <c r="D59" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
+      <c r="B61" t="s">
         <v>206</v>
       </c>
-      <c r="B60" t="s">
+      <c r="C61" t="s">
         <v>207</v>
       </c>
-      <c r="C60" t="s">
+      <c r="D61" t="s">
         <v>208</v>
       </c>
-      <c r="D60" t="s">
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
+      <c r="B62" t="s">
         <v>210</v>
       </c>
-      <c r="B61" t="s">
+      <c r="C62" t="s">
         <v>211</v>
       </c>
-      <c r="C61" t="s">
+      <c r="D62" t="s">
         <v>212</v>
       </c>
-      <c r="D61" t="s">
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
+      <c r="B63" t="s">
         <v>214</v>
       </c>
-      <c r="B62" t="s">
+      <c r="C63" t="s">
         <v>215</v>
       </c>
-      <c r="C62" t="s">
+      <c r="D63" t="s">
         <v>216</v>
       </c>
-      <c r="D62" t="s">
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
+      <c r="B64" t="s">
+        <v>214</v>
+      </c>
+      <c r="C64" t="s">
         <v>218</v>
       </c>
-      <c r="B63" t="s">
+      <c r="D64" t="s">
         <v>219</v>
       </c>
-      <c r="C63" t="s">
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
         <v>220</v>
       </c>
-      <c r="D63" t="s">
+      <c r="B65" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
+      <c r="C65" t="s">
         <v>222</v>
       </c>
-      <c r="B64" t="s">
-        <v>219</v>
-      </c>
-      <c r="C64" t="s">
+      <c r="D65" t="s">
         <v>223</v>
       </c>
-      <c r="D64" t="s">
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
+      <c r="B66" t="s">
+        <v>221</v>
+      </c>
+      <c r="C66" t="s">
         <v>225</v>
       </c>
-      <c r="B65" t="s">
+      <c r="D66" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
         <v>226</v>
       </c>
-      <c r="C65" t="s">
+      <c r="B67" t="s">
+        <v>221</v>
+      </c>
+      <c r="C67" t="s">
         <v>227</v>
       </c>
-      <c r="D65" t="s">
+      <c r="D67" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
+      <c r="B68" t="s">
         <v>229</v>
       </c>
-      <c r="B66" t="s">
-        <v>226</v>
-      </c>
-      <c r="C66" t="s">
+      <c r="C68" t="s">
         <v>230</v>
       </c>
-      <c r="D66" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
+      <c r="D68" t="s">
         <v>231</v>
       </c>
-      <c r="B67" t="s">
-        <v>226</v>
-      </c>
-      <c r="C67" t="s">
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
         <v>232</v>
       </c>
-      <c r="D67" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
+      <c r="B69" t="s">
+        <v>229</v>
+      </c>
+      <c r="C69" t="s">
         <v>233</v>
       </c>
-      <c r="B68" t="s">
+      <c r="D69" t="s">
         <v>234</v>
       </c>
-      <c r="C68" t="s">
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
         <v>235</v>
       </c>
-      <c r="D68" t="s">
+      <c r="B70" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
+      <c r="C70" t="s">
         <v>237</v>
       </c>
-      <c r="B69" t="s">
-        <v>234</v>
-      </c>
-      <c r="C69" t="s">
+      <c r="D70" t="s">
         <v>238</v>
       </c>
-      <c r="D69" t="s">
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
+      <c r="B71" t="s">
         <v>240</v>
       </c>
-      <c r="B70" t="s">
+      <c r="C71" t="s">
         <v>241</v>
       </c>
-      <c r="C70" t="s">
+      <c r="D71" t="s">
         <v>242</v>
       </c>
-      <c r="D70" t="s">
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="71" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
+      <c r="B72" t="s">
         <v>244</v>
       </c>
-      <c r="B71" t="s">
+      <c r="C72" t="s">
         <v>245</v>
       </c>
-      <c r="C71" t="s">
+      <c r="D72" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
         <v>246</v>
       </c>
-      <c r="D71" t="s">
+      <c r="B73" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="72" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
+      <c r="C73" t="s">
         <v>248</v>
       </c>
-      <c r="B72" t="s">
+      <c r="D73" t="s">
         <v>249</v>
       </c>
-      <c r="C72" t="s">
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
         <v>250</v>
       </c>
-      <c r="D72" t="s">
+      <c r="B74" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="73" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
+      <c r="C74" t="s">
         <v>252</v>
       </c>
-      <c r="B73" t="s">
+      <c r="D74" t="s">
         <v>253</v>
       </c>
-      <c r="C73" t="s">
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
         <v>254</v>
       </c>
-      <c r="D73" t="s">
+      <c r="B75" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="74" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
+      <c r="C75" t="s">
         <v>256</v>
       </c>
-      <c r="B74" t="s">
+      <c r="D75" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
         <v>257</v>
       </c>
-      <c r="C74" t="s">
+      <c r="B76" t="s">
         <v>258</v>
       </c>
-      <c r="D74" t="s">
+      <c r="C76" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="75" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
+      <c r="D76" t="s">
         <v>260</v>
       </c>
-      <c r="B75" t="s">
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
         <v>261</v>
       </c>
-      <c r="C75" t="s">
+      <c r="B77" t="s">
         <v>262</v>
       </c>
-      <c r="D75" t="s">
+      <c r="C77" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="76" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
+      <c r="D77" t="s">
         <v>264</v>
       </c>
-      <c r="B76" t="s">
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
         <v>265</v>
       </c>
-      <c r="C76" t="s">
+      <c r="B78" t="s">
         <v>266</v>
       </c>
-      <c r="D76" t="s">
+      <c r="C78" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="77" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
+      <c r="D78" t="s">
         <v>268</v>
       </c>
-      <c r="B77" t="s">
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
         <v>269</v>
       </c>
-      <c r="C77" t="s">
+      <c r="B79" t="s">
         <v>270</v>
       </c>
-      <c r="D77" t="s">
+      <c r="C79" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="78" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
+      <c r="D79" t="s">
         <v>272</v>
       </c>
-      <c r="B78" t="s">
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
         <v>273</v>
       </c>
-      <c r="C78" t="s">
+      <c r="B80" t="s">
         <v>274</v>
       </c>
-      <c r="D78" t="s">
+      <c r="C80" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="79" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
+      <c r="D80" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
         <v>276</v>
       </c>
-      <c r="B79" t="s">
+      <c r="B81" t="s">
+        <v>274</v>
+      </c>
+      <c r="C81" t="s">
         <v>277</v>
       </c>
-      <c r="C79" t="s">
+      <c r="D81" t="s">
         <v>278</v>
       </c>
-      <c r="D79" t="s">
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="80" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
+      <c r="B82" t="s">
         <v>280</v>
       </c>
-      <c r="B80" t="s">
+      <c r="C82" t="s">
         <v>281</v>
       </c>
-      <c r="C80" t="s">
+      <c r="D82" t="s">
         <v>282</v>
       </c>
-      <c r="D80" t="s">
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
         <v>283</v>
       </c>
-    </row>
-    <row r="81" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
+      <c r="B83" t="s">
         <v>284</v>
       </c>
-      <c r="B81" t="s">
-        <v>281</v>
-      </c>
-      <c r="C81" t="s">
+      <c r="C83" t="s">
         <v>285</v>
       </c>
-      <c r="D81" t="s">
+      <c r="D83" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="82" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
         <v>287</v>
       </c>
-      <c r="B82" t="s">
+      <c r="B84" t="s">
         <v>288</v>
       </c>
-      <c r="C82" t="s">
+      <c r="C84" t="s">
         <v>289</v>
       </c>
-      <c r="D82" t="s">
+      <c r="D84" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="83" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
         <v>291</v>
       </c>
-      <c r="B83" t="s">
+      <c r="B85" t="s">
         <v>292</v>
       </c>
-      <c r="C83" t="s">
+      <c r="C85" t="s">
         <v>293</v>
       </c>
-      <c r="D83" t="s">
+      <c r="D85" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="84" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
+      <c r="B86" t="s">
         <v>295</v>
       </c>
-      <c r="B84" t="s">
+      <c r="C86" t="s">
         <v>296</v>
       </c>
-      <c r="C84" t="s">
+      <c r="D86" t="s">
         <v>297</v>
       </c>
-      <c r="D84" t="s">
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="85" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
+      <c r="B87" t="s">
         <v>299</v>
       </c>
-      <c r="B85" t="s">
+      <c r="C87" t="s">
         <v>300</v>
       </c>
-      <c r="C85" t="s">
+      <c r="D87" t="s">
         <v>301</v>
       </c>
-      <c r="D85" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
         <v>302</v>
       </c>
-      <c r="B86" t="s">
+      <c r="B88" t="s">
         <v>303</v>
       </c>
-      <c r="C86" t="s">
+      <c r="C88" t="s">
         <v>304</v>
       </c>
-      <c r="D86" t="s">
+      <c r="D88" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="87" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
         <v>306</v>
       </c>
-      <c r="B87" t="s">
+      <c r="B89" t="s">
         <v>307</v>
       </c>
-      <c r="C87" t="s">
+      <c r="C89" t="s">
         <v>308</v>
       </c>
-      <c r="D87" t="s">
+      <c r="D89" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="88" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
         <v>310</v>
       </c>
-      <c r="B88" t="s">
+      <c r="B90" t="s">
         <v>311</v>
       </c>
-      <c r="C88" t="s">
+      <c r="C90" t="s">
         <v>312</v>
       </c>
-      <c r="D88" t="s">
+      <c r="D90" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="89" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
         <v>314</v>
       </c>
-      <c r="B89" t="s">
+      <c r="B91" t="s">
         <v>315</v>
       </c>
-      <c r="C89" t="s">
+      <c r="C91" t="s">
         <v>316</v>
       </c>
-      <c r="D89" t="s">
+      <c r="D91" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="90" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
         <v>318</v>
       </c>
-      <c r="B90" t="s">
+      <c r="B92" t="s">
         <v>319</v>
       </c>
-      <c r="C90" t="s">
+      <c r="C92" t="s">
         <v>320</v>
       </c>
-      <c r="D90" t="s">
+      <c r="D92" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="91" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
         <v>322</v>
       </c>
-      <c r="B91" t="s">
+      <c r="B93" t="s">
         <v>323</v>
       </c>
-      <c r="C91" t="s">
+      <c r="C93" t="s">
         <v>324</v>
       </c>
-      <c r="D91" t="s">
+      <c r="D93" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="92" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
         <v>326</v>
       </c>
-      <c r="B92" t="s">
+      <c r="B94" t="s">
         <v>327</v>
       </c>
-      <c r="C92" t="s">
+      <c r="C94" t="s">
         <v>328</v>
       </c>
-      <c r="D92" t="s">
+      <c r="D94" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="93" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A93" t="s">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
         <v>330</v>
       </c>
-      <c r="B93" t="s">
+      <c r="B95" t="s">
         <v>331</v>
       </c>
-      <c r="C93" t="s">
+      <c r="C95" t="s">
         <v>332</v>
       </c>
-      <c r="D93" t="s">
+      <c r="D95" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="94" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
         <v>334</v>
       </c>
-      <c r="B94" t="s">
+      <c r="B96" t="s">
         <v>335</v>
       </c>
-      <c r="C94" t="s">
+      <c r="C96" t="s">
         <v>336</v>
       </c>
-      <c r="D94" t="s">
+      <c r="D96" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="95" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
         <v>338</v>
       </c>
-      <c r="B95" t="s">
+      <c r="B97" t="s">
         <v>339</v>
       </c>
-      <c r="C95" t="s">
+      <c r="C97" t="s">
         <v>340</v>
       </c>
-      <c r="D95" t="s">
+      <c r="D97" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="96" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A96" t="s">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
         <v>342</v>
       </c>
-      <c r="B96" t="s">
+      <c r="B98" t="s">
         <v>343</v>
       </c>
-      <c r="C96" t="s">
+      <c r="C98" t="s">
         <v>344</v>
       </c>
-      <c r="D96" t="s">
+      <c r="D98" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="97" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A97" t="s">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
         <v>346</v>
       </c>
-      <c r="B97" t="s">
+      <c r="B99" t="s">
         <v>347</v>
       </c>
-      <c r="C97" t="s">
+      <c r="C99" t="s">
         <v>348</v>
       </c>
-      <c r="D97" t="s">
+      <c r="D99" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
         <v>349</v>
       </c>
-    </row>
-    <row r="98" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A98" t="s">
+      <c r="B100" t="s">
         <v>350</v>
       </c>
-      <c r="B98" t="s">
+      <c r="C100" t="s">
         <v>351</v>
       </c>
-      <c r="C98" t="s">
+      <c r="D100" t="s">
         <v>352</v>
       </c>
-      <c r="D98" t="s">
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
         <v>353</v>
       </c>
-    </row>
-    <row r="99" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A99" t="s">
+      <c r="B101" t="s">
         <v>354</v>
       </c>
-      <c r="B99" t="s">
+      <c r="C101" t="s">
         <v>355</v>
       </c>
-      <c r="C99" t="s">
+      <c r="D101" t="s">
         <v>356</v>
       </c>
-      <c r="D99" t="s">
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A102" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="100" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A100" t="s">
+      <c r="B102" t="s">
         <v>358</v>
       </c>
-      <c r="B100" t="s">
+      <c r="C102" t="s">
         <v>359</v>
       </c>
-      <c r="C100" t="s">
+      <c r="D102" t="s">
         <v>360</v>
       </c>
-      <c r="D100" t="s">
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A103" t="s">
         <v>361</v>
       </c>
-    </row>
-    <row r="101" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A101" t="s">
+      <c r="B103" t="s">
         <v>362</v>
       </c>
-      <c r="B101" t="s">
+      <c r="C103" t="s">
         <v>363</v>
       </c>
-      <c r="C101" t="s">
+      <c r="D103" t="s">
         <v>364</v>
       </c>
-      <c r="D101" t="s">
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
         <v>365</v>
       </c>
-    </row>
-    <row r="102" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A102" t="s">
+      <c r="B104" t="s">
         <v>366</v>
       </c>
-      <c r="B102" t="s">
+      <c r="C104" t="s">
         <v>367</v>
       </c>
-      <c r="C102" t="s">
+      <c r="D104" t="s">
         <v>368</v>
       </c>
-      <c r="D102" t="s">
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A105" t="s">
         <v>369</v>
       </c>
-    </row>
-    <row r="103" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A103" t="s">
+      <c r="B105" t="s">
         <v>370</v>
       </c>
-      <c r="B103" t="s">
+      <c r="C105" t="s">
         <v>371</v>
       </c>
-      <c r="C103" t="s">
+      <c r="D105" t="s">
         <v>372</v>
       </c>
-      <c r="D103" t="s">
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A106" t="s">
         <v>373</v>
       </c>
-    </row>
-    <row r="104" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A104" t="s">
+      <c r="B106" t="s">
         <v>374</v>
       </c>
-      <c r="B104" t="s">
+      <c r="C106" t="s">
         <v>375</v>
       </c>
-      <c r="C104" t="s">
+      <c r="D106" t="s">
         <v>376</v>
       </c>
-      <c r="D104" t="s">
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A107" t="s">
         <v>377</v>
       </c>
-    </row>
-    <row r="105" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A105" t="s">
+      <c r="B107" t="s">
         <v>378</v>
       </c>
-      <c r="B105" t="s">
+      <c r="C107" t="s">
         <v>379</v>
       </c>
-      <c r="C105" t="s">
+      <c r="D107" t="s">
         <v>380</v>
       </c>
-      <c r="D105" t="s">
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A108" t="s">
         <v>381</v>
       </c>
-    </row>
-    <row r="106" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A106" t="s">
+      <c r="B108" t="s">
         <v>382</v>
       </c>
-      <c r="B106" t="s">
+      <c r="C108" t="s">
         <v>383</v>
       </c>
-      <c r="C106" t="s">
+      <c r="D108" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A109" t="s">
         <v>384</v>
       </c>
-      <c r="D106" t="s">
+      <c r="B109" t="s">
         <v>385</v>
       </c>
-    </row>
-    <row r="107" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A107" t="s">
+      <c r="C109" t="s">
         <v>386</v>
       </c>
-      <c r="B107" t="s">
+      <c r="D109" t="s">
         <v>387</v>
       </c>
-      <c r="C107" t="s">
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A110" t="s">
         <v>388</v>
       </c>
-      <c r="D107" t="s">
+      <c r="B110" t="s">
         <v>389</v>
       </c>
-    </row>
-    <row r="108" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A108" t="s">
+      <c r="C110" t="s">
         <v>390</v>
       </c>
-      <c r="B108" t="s">
+      <c r="D110" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A111" t="s">
         <v>391</v>
       </c>
-      <c r="C108" t="s">
+      <c r="B111" t="s">
+        <v>389</v>
+      </c>
+      <c r="C111" t="s">
+        <v>390</v>
+      </c>
+      <c r="D111" t="s">
         <v>392</v>
       </c>
-      <c r="D108" t="s">
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A112" t="s">
         <v>393</v>
       </c>
-    </row>
-    <row r="109" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A109" t="s">
+      <c r="B112" t="s">
         <v>394</v>
       </c>
-      <c r="B109" t="s">
+      <c r="C112" t="s">
         <v>395</v>
       </c>
-      <c r="C109" t="s">
+      <c r="D112" t="s">
         <v>396</v>
       </c>
-      <c r="D109" t="s">
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A113" t="s">
         <v>397</v>
       </c>
-    </row>
-    <row r="110" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A110" t="s">
+      <c r="B113" t="s">
+        <v>394</v>
+      </c>
+      <c r="C113" t="s">
         <v>398</v>
       </c>
-      <c r="B110" t="s">
+      <c r="D113" t="s">
         <v>399</v>
       </c>
-      <c r="C110" t="s">
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A114" t="s">
         <v>400</v>
       </c>
-      <c r="D110" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="111" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A111" t="s">
+      <c r="B114" t="s">
         <v>401</v>
       </c>
-      <c r="B111" t="s">
-        <v>399</v>
-      </c>
-      <c r="C111" t="s">
-        <v>400</v>
-      </c>
-      <c r="D111" t="s">
+      <c r="C114" t="s">
         <v>402</v>
       </c>
-    </row>
-    <row r="112" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A112" t="s">
+      <c r="D114" t="s">
         <v>403</v>
       </c>
-      <c r="B112" t="s">
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A115" t="s">
         <v>404</v>
       </c>
-      <c r="C112" t="s">
+      <c r="B115" t="s">
         <v>405</v>
       </c>
-      <c r="D112" t="s">
+      <c r="C115" t="s">
+        <v>99</v>
+      </c>
+      <c r="D115" t="s">
         <v>406</v>
       </c>
     </row>
-    <row r="113" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A113" t="s">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A116" t="s">
         <v>407</v>
       </c>
-      <c r="B113" t="s">
-        <v>404</v>
-      </c>
-      <c r="C113" t="s">
+      <c r="B116" t="s">
         <v>408</v>
       </c>
-      <c r="D113" t="s">
+      <c r="C116" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="114" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A114" t="s">
+      <c r="D116" t="s">
         <v>410</v>
       </c>
-      <c r="B114" t="s">
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A117" t="s">
         <v>411</v>
       </c>
-      <c r="C114" t="s">
+      <c r="B117" t="s">
         <v>412</v>
       </c>
-      <c r="D114" t="s">
+      <c r="C117" t="s">
         <v>413</v>
       </c>
-    </row>
-    <row r="115" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A115" t="s">
+      <c r="D117" t="s">
         <v>414</v>
       </c>
-      <c r="B115" t="s">
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A118" t="s">
         <v>415</v>
       </c>
-      <c r="C115" t="s">
-        <v>102</v>
-      </c>
-      <c r="D115" t="s">
+      <c r="B118" t="s">
         <v>416</v>
       </c>
-    </row>
-    <row r="116" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A116" t="s">
+      <c r="C118" t="s">
         <v>417</v>
       </c>
-      <c r="B116" t="s">
+      <c r="D118" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A119" t="s">
         <v>418</v>
       </c>
-      <c r="C116" t="s">
+      <c r="B119" t="s">
+        <v>416</v>
+      </c>
+      <c r="C119" t="s">
         <v>419</v>
       </c>
-      <c r="D116" t="s">
+      <c r="D119" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A120" t="s">
         <v>420</v>
       </c>
-    </row>
-    <row r="117" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A117" t="s">
+      <c r="B120" t="s">
+        <v>416</v>
+      </c>
+      <c r="C120" t="s">
         <v>421</v>
       </c>
-      <c r="B117" t="s">
+      <c r="D120" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A121" t="s">
         <v>422</v>
       </c>
-      <c r="C117" t="s">
+      <c r="B121" t="s">
+        <v>416</v>
+      </c>
+      <c r="C121" t="s">
         <v>423</v>
       </c>
-      <c r="D117" t="s">
+      <c r="D121" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A122" t="s">
         <v>424</v>
       </c>
-    </row>
-    <row r="118" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A118" t="s">
+      <c r="B122" t="s">
         <v>425</v>
       </c>
-      <c r="B118" t="s">
+      <c r="C122" t="s">
         <v>426</v>
       </c>
-      <c r="C118" t="s">
+      <c r="D122" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A123" t="s">
         <v>427</v>
       </c>
-      <c r="D118" t="s">
+      <c r="B123" t="s">
         <v>428</v>
       </c>
-    </row>
-    <row r="119" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A119" t="s">
+      <c r="C123" t="s">
         <v>429</v>
       </c>
-      <c r="B119" t="s">
-        <v>426</v>
-      </c>
-      <c r="C119" t="s">
+      <c r="D123" t="s">
         <v>430</v>
       </c>
-      <c r="D119" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="120" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A120" t="s">
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A124" t="s">
         <v>431</v>
       </c>
-      <c r="B120" t="s">
-        <v>426</v>
-      </c>
-      <c r="C120" t="s">
+      <c r="B124" t="s">
         <v>432</v>
       </c>
-      <c r="D120" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="121" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A121" t="s">
+      <c r="C124" t="s">
         <v>433</v>
       </c>
-      <c r="B121" t="s">
-        <v>426</v>
-      </c>
-      <c r="C121" t="s">
+      <c r="D124" t="s">
         <v>434</v>
       </c>
-      <c r="D121" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="122" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A122" t="s">
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A125" t="s">
         <v>435</v>
       </c>
-      <c r="B122" t="s">
+      <c r="B125" t="s">
         <v>436</v>
       </c>
-      <c r="C122" t="s">
+      <c r="C125" t="s">
         <v>437</v>
       </c>
-      <c r="D122" t="s">
+      <c r="D125" t="s">
         <v>438</v>
       </c>
     </row>
-    <row r="123" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A123" t="s">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A126" t="s">
         <v>439</v>
       </c>
-      <c r="B123" t="s">
+      <c r="B126" t="s">
         <v>440</v>
       </c>
-      <c r="C123" t="s">
+      <c r="C126" t="s">
         <v>441</v>
       </c>
-      <c r="D123" t="s">
+      <c r="D126" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A127" t="s">
         <v>442</v>
       </c>
-    </row>
-    <row r="124" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A124" t="s">
+      <c r="B127" t="s">
         <v>443</v>
       </c>
-      <c r="B124" t="s">
+      <c r="C127" t="s">
         <v>444</v>
       </c>
-      <c r="C124" t="s">
+      <c r="D127" t="s">
         <v>445</v>
       </c>
-      <c r="D124" t="s">
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A128" t="s">
         <v>446</v>
       </c>
-    </row>
-    <row r="125" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A125" t="s">
+      <c r="B128" t="s">
         <v>447</v>
       </c>
-      <c r="B125" t="s">
+      <c r="C128" t="s">
         <v>448</v>
       </c>
-      <c r="C125" t="s">
+      <c r="D128" t="s">
         <v>449</v>
       </c>
-      <c r="D125" t="s">
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A129" t="s">
         <v>450</v>
       </c>
-    </row>
-    <row r="126" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A126" t="s">
+      <c r="B129" t="s">
         <v>451</v>
       </c>
-      <c r="B126" t="s">
+      <c r="C129" t="s">
         <v>452</v>
       </c>
-      <c r="C126" t="s">
+      <c r="D129" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A130" t="s">
         <v>453</v>
       </c>
-      <c r="D126" t="s">
+      <c r="B130" t="s">
         <v>454</v>
       </c>
-    </row>
-    <row r="127" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A127" t="s">
+      <c r="C130" t="s">
         <v>455</v>
       </c>
-      <c r="B127" t="s">
+      <c r="D130" t="s">
         <v>456</v>
       </c>
-      <c r="C127" t="s">
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A131" t="s">
         <v>457</v>
       </c>
-      <c r="D127" t="s">
+      <c r="B131" t="s">
+        <v>454</v>
+      </c>
+      <c r="C131" t="s">
         <v>458</v>
       </c>
-    </row>
-    <row r="128" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A128" t="s">
+      <c r="D131" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A132" t="s">
         <v>459</v>
       </c>
-      <c r="B128" t="s">
+      <c r="B132" t="s">
         <v>460</v>
       </c>
-      <c r="C128" t="s">
+      <c r="C132" t="s">
         <v>461</v>
       </c>
-      <c r="D128" t="s">
+      <c r="D132" t="s">
         <v>462</v>
       </c>
     </row>
-    <row r="129" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A129" t="s">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A133" t="s">
         <v>463</v>
       </c>
-      <c r="B129" t="s">
+      <c r="B133" t="s">
         <v>464</v>
       </c>
-      <c r="C129" t="s">
+      <c r="C133" t="s">
         <v>465</v>
       </c>
-      <c r="D129" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="130" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A130" t="s">
+      <c r="D133" t="s">
         <v>466</v>
       </c>
-      <c r="B130" t="s">
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A134" t="s">
         <v>467</v>
       </c>
-      <c r="C130" t="s">
+      <c r="B134" t="s">
+        <v>464</v>
+      </c>
+      <c r="C134" t="s">
         <v>468</v>
       </c>
-      <c r="D130" t="s">
+      <c r="D134" t="s">
         <v>469</v>
       </c>
     </row>
-    <row r="131" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A131" t="s">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A135" t="s">
         <v>470</v>
       </c>
-      <c r="B131" t="s">
-        <v>467</v>
-      </c>
-      <c r="C131" t="s">
+      <c r="B135" t="s">
         <v>471</v>
-      </c>
-      <c r="D131" t="s">
-        <v>469</v>
-      </c>
-    </row>
-    <row r="132" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A132" t="s">
-        <v>472</v>
-      </c>
-      <c r="B132" t="s">
-        <v>473</v>
-      </c>
-      <c r="C132" t="s">
-        <v>474</v>
-      </c>
-      <c r="D132" t="s">
-        <v>475</v>
-      </c>
-    </row>
-    <row r="133" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A133" t="s">
-        <v>476</v>
-      </c>
-      <c r="B133" t="s">
-        <v>477</v>
-      </c>
-      <c r="C133" t="s">
-        <v>478</v>
-      </c>
-      <c r="D133" t="s">
-        <v>479</v>
-      </c>
-    </row>
-    <row r="134" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A134" t="s">
-        <v>480</v>
-      </c>
-      <c r="B134" t="s">
-        <v>477</v>
-      </c>
-      <c r="C134" t="s">
-        <v>481</v>
-      </c>
-      <c r="D134" t="s">
-        <v>482</v>
-      </c>
-    </row>
-    <row r="135" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A135" t="s">
-        <v>483</v>
-      </c>
-      <c r="B135" t="s">
-        <v>484</v>
       </c>
       <c r="C135" t="s">
         <v>10</v>
       </c>
       <c r="D135" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="136" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
+        <v>472</v>
+      </c>
+      <c r="B136" t="s">
+        <v>473</v>
+      </c>
+      <c r="C136" t="s">
+        <v>474</v>
+      </c>
+      <c r="D136" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A137" t="s">
+        <v>476</v>
+      </c>
+      <c r="B137" t="s">
+        <v>477</v>
+      </c>
+      <c r="C137" t="s">
+        <v>478</v>
+      </c>
+      <c r="D137" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A138" t="s">
+        <v>480</v>
+      </c>
+      <c r="B138" t="s">
+        <v>481</v>
+      </c>
+      <c r="C138" t="s">
+        <v>482</v>
+      </c>
+      <c r="D138" t="s">
         <v>485</v>
       </c>
-      <c r="B136" t="s">
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A139" t="s">
+        <v>483</v>
+      </c>
+      <c r="B139" t="s">
+        <v>481</v>
+      </c>
+      <c r="C139" t="s">
+        <v>484</v>
+      </c>
+      <c r="D139" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A140" t="s">
         <v>486</v>
       </c>
-      <c r="C136" t="s">
+      <c r="B140" t="s">
         <v>487</v>
       </c>
-      <c r="D136" t="s">
+      <c r="C140" t="s">
         <v>488</v>
       </c>
-    </row>
-    <row r="137" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A137" t="s">
+      <c r="D140" t="s">
         <v>489</v>
       </c>
-      <c r="B137" t="s">
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A141" t="s">
         <v>490</v>
       </c>
-      <c r="C137" t="s">
+      <c r="B141" t="s">
         <v>491</v>
       </c>
-      <c r="D137" t="s">
+      <c r="C141" t="s">
         <v>492</v>
       </c>
-    </row>
-    <row r="138" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A138" t="s">
+      <c r="D141" t="s">
         <v>493</v>
       </c>
-      <c r="B138" t="s">
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A142" t="s">
         <v>494</v>
       </c>
-      <c r="C138" t="s">
+      <c r="B142" t="s">
         <v>495</v>
       </c>
-      <c r="D138" t="s">
+      <c r="C142" t="s">
         <v>496</v>
       </c>
-    </row>
-    <row r="139" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A139" t="s">
+      <c r="D142" t="s">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A143" t="s">
         <v>497</v>
       </c>
-      <c r="B139" t="s">
-        <v>494</v>
-      </c>
-      <c r="C139" t="s">
+      <c r="B143" t="s">
         <v>498</v>
       </c>
-      <c r="D139" t="s">
+      <c r="C143" t="s">
         <v>499</v>
       </c>
-    </row>
-    <row r="140" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A140" t="s">
+      <c r="D143" t="s">
         <v>500</v>
       </c>
-      <c r="B140" t="s">
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A144" t="s">
         <v>501</v>
       </c>
-      <c r="C140" t="s">
+      <c r="B144" t="s">
         <v>502</v>
       </c>
-      <c r="D140" t="s">
+      <c r="C144" t="s">
         <v>503</v>
       </c>
-    </row>
-    <row r="141" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A141" t="s">
+      <c r="D144" t="s">
         <v>504</v>
       </c>
-      <c r="B141" t="s">
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A145" t="s">
         <v>505</v>
       </c>
-      <c r="C141" t="s">
+      <c r="B145" t="s">
         <v>506</v>
-      </c>
-      <c r="D141" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="142" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A142" t="s">
-        <v>508</v>
-      </c>
-      <c r="B142" t="s">
-        <v>509</v>
-      </c>
-      <c r="C142" t="s">
-        <v>510</v>
-      </c>
-      <c r="D142" t="s">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="143" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A143" t="s">
-        <v>512</v>
-      </c>
-      <c r="B143" t="s">
-        <v>513</v>
-      </c>
-      <c r="C143" t="s">
-        <v>514</v>
-      </c>
-      <c r="D143" t="s">
-        <v>515</v>
-      </c>
-    </row>
-    <row r="144" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A144" t="s">
-        <v>516</v>
-      </c>
-      <c r="B144" t="s">
-        <v>517</v>
-      </c>
-      <c r="C144" t="s">
-        <v>518</v>
-      </c>
-      <c r="D144" t="s">
-        <v>519</v>
-      </c>
-    </row>
-    <row r="145" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A145" t="s">
-        <v>520</v>
-      </c>
-      <c r="B145" t="s">
-        <v>521</v>
       </c>
       <c r="C145" t="s">
         <v>10</v>
       </c>
       <c r="D145" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="146" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
+        <v>507</v>
+      </c>
+      <c r="B146" t="s">
+        <v>508</v>
+      </c>
+      <c r="C146" t="s">
+        <v>509</v>
+      </c>
+      <c r="D146" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A147" t="s">
+        <v>511</v>
+      </c>
+      <c r="B147" t="s">
+        <v>512</v>
+      </c>
+      <c r="C147" t="s">
+        <v>513</v>
+      </c>
+      <c r="D147" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A148" t="s">
+        <v>514</v>
+      </c>
+      <c r="B148" t="s">
+        <v>515</v>
+      </c>
+      <c r="C148" t="s">
+        <v>516</v>
+      </c>
+      <c r="D148" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A149" t="s">
+        <v>518</v>
+      </c>
+      <c r="B149" t="s">
+        <v>519</v>
+      </c>
+      <c r="C149" t="s">
+        <v>520</v>
+      </c>
+      <c r="D149" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A150" t="s">
         <v>522</v>
       </c>
-      <c r="B146" t="s">
+      <c r="B150" t="s">
         <v>523</v>
       </c>
-      <c r="C146" t="s">
+      <c r="C150" t="s">
         <v>524</v>
       </c>
-      <c r="D146" t="s">
+      <c r="D150" t="s">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A151" t="s">
         <v>525</v>
       </c>
-    </row>
-    <row r="147" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A147" t="s">
+      <c r="B151" t="s">
         <v>526</v>
       </c>
-      <c r="B147" t="s">
+      <c r="C151" t="s">
         <v>527</v>
       </c>
-      <c r="C147" t="s">
+      <c r="D151" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A152" t="s">
         <v>528</v>
       </c>
-      <c r="D147" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="148" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A148" t="s">
+      <c r="B152" t="s">
         <v>529</v>
       </c>
-      <c r="B148" t="s">
+      <c r="C152" t="s">
         <v>530</v>
       </c>
-      <c r="C148" t="s">
+      <c r="D152" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A153" t="s">
         <v>531</v>
       </c>
-      <c r="D148" t="s">
+      <c r="B153" t="s">
         <v>532</v>
       </c>
-    </row>
-    <row r="149" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A149" t="s">
+      <c r="C153" t="s">
         <v>533</v>
       </c>
-      <c r="B149" t="s">
+      <c r="D153" t="s">
         <v>534</v>
       </c>
-      <c r="C149" t="s">
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A154" t="s">
         <v>535</v>
       </c>
-      <c r="D149" t="s">
+      <c r="B154" t="s">
         <v>536</v>
       </c>
-    </row>
-    <row r="150" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A150" t="s">
+      <c r="C154" t="s">
+        <v>101</v>
+      </c>
+      <c r="D154" t="s">
         <v>537</v>
       </c>
-      <c r="B150" t="s">
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A155" t="s">
         <v>538</v>
       </c>
-      <c r="C150" t="s">
+      <c r="B155" t="s">
         <v>539</v>
       </c>
-      <c r="D150" t="s">
+      <c r="C155" t="s">
         <v>540</v>
       </c>
-    </row>
-    <row r="151" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A151" t="s">
+      <c r="D155" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A156" t="s">
         <v>541</v>
       </c>
-      <c r="B151" t="s">
+      <c r="B156" t="s">
         <v>542</v>
       </c>
-      <c r="C151" t="s">
+      <c r="C156" t="s">
         <v>543</v>
       </c>
-      <c r="D151" t="s">
+      <c r="D156" t="s">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A157" t="s">
         <v>544</v>
       </c>
-    </row>
-    <row r="152" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A152" t="s">
+      <c r="B157" t="s">
         <v>545</v>
       </c>
-      <c r="B152" t="s">
+      <c r="C157" t="s">
         <v>546</v>
       </c>
-      <c r="C152" t="s">
+      <c r="D157" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A158" t="s">
         <v>547</v>
       </c>
-      <c r="D152" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="153" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A153" t="s">
+      <c r="B158" t="s">
         <v>548</v>
       </c>
-      <c r="B153" t="s">
+      <c r="C158" t="s">
         <v>549</v>
       </c>
-      <c r="C153" t="s">
+      <c r="D158" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A159" t="s">
         <v>550</v>
       </c>
-      <c r="D153" t="s">
+      <c r="B159" t="s">
         <v>551</v>
-      </c>
-    </row>
-    <row r="154" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A154" t="s">
-        <v>552</v>
-      </c>
-      <c r="B154" t="s">
-        <v>553</v>
-      </c>
-      <c r="C154" t="s">
-        <v>104</v>
-      </c>
-      <c r="D154" t="s">
-        <v>554</v>
-      </c>
-    </row>
-    <row r="155" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A155" t="s">
-        <v>555</v>
-      </c>
-      <c r="B155" t="s">
-        <v>556</v>
-      </c>
-      <c r="C155" t="s">
-        <v>557</v>
-      </c>
-      <c r="D155" t="s">
-        <v>558</v>
-      </c>
-    </row>
-    <row r="156" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A156" t="s">
-        <v>559</v>
-      </c>
-      <c r="B156" t="s">
-        <v>560</v>
-      </c>
-      <c r="C156" t="s">
-        <v>561</v>
-      </c>
-      <c r="D156" t="s">
-        <v>562</v>
-      </c>
-    </row>
-    <row r="157" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A157" t="s">
-        <v>563</v>
-      </c>
-      <c r="B157" t="s">
-        <v>564</v>
-      </c>
-      <c r="C157" t="s">
-        <v>565</v>
-      </c>
-      <c r="D157" t="s">
-        <v>566</v>
-      </c>
-    </row>
-    <row r="158" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A158" t="s">
-        <v>567</v>
-      </c>
-      <c r="B158" t="s">
-        <v>568</v>
-      </c>
-      <c r="C158" t="s">
-        <v>569</v>
-      </c>
-      <c r="D158" t="s">
-        <v>570</v>
-      </c>
-    </row>
-    <row r="159" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A159" t="s">
-        <v>571</v>
-      </c>
-      <c r="B159" t="s">
-        <v>572</v>
       </c>
       <c r="C159" t="s">
         <v>10</v>
       </c>
       <c r="D159" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="160" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
+        <v>552</v>
+      </c>
+      <c r="B160" t="s">
+        <v>553</v>
+      </c>
+      <c r="C160" t="s">
+        <v>554</v>
+      </c>
+      <c r="D160" t="s">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A161" t="s">
+        <v>555</v>
+      </c>
+      <c r="B161" t="s">
+        <v>553</v>
+      </c>
+      <c r="C161" t="s">
+        <v>556</v>
+      </c>
+      <c r="D161" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A162" t="s">
+        <v>557</v>
+      </c>
+      <c r="B162" t="s">
+        <v>558</v>
+      </c>
+      <c r="C162" t="s">
+        <v>559</v>
+      </c>
+      <c r="D162" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A163" t="s">
+        <v>561</v>
+      </c>
+      <c r="B163" t="s">
+        <v>562</v>
+      </c>
+      <c r="C163" t="s">
+        <v>563</v>
+      </c>
+      <c r="D163" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A164" t="s">
+        <v>564</v>
+      </c>
+      <c r="B164" t="s">
+        <v>565</v>
+      </c>
+      <c r="C164" t="s">
+        <v>566</v>
+      </c>
+      <c r="D164" t="s">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A165" t="s">
+        <v>567</v>
+      </c>
+      <c r="B165" t="s">
+        <v>568</v>
+      </c>
+      <c r="C165" t="s">
+        <v>569</v>
+      </c>
+      <c r="D165" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A166" t="s">
+        <v>570</v>
+      </c>
+      <c r="B166" t="s">
+        <v>571</v>
+      </c>
+      <c r="C166" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A167" t="s">
         <v>573</v>
       </c>
-      <c r="B160" t="s">
+      <c r="B167" t="s">
         <v>574</v>
       </c>
-      <c r="C160" t="s">
+      <c r="C167" t="s">
         <v>575</v>
       </c>
-      <c r="D160" t="s">
+      <c r="D167" t="s">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A168" t="s">
         <v>576</v>
       </c>
-    </row>
-    <row r="161" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A161" t="s">
+      <c r="B168" t="s">
         <v>577</v>
       </c>
-      <c r="B161" t="s">
-        <v>574</v>
-      </c>
-      <c r="C161" t="s">
+      <c r="C168" t="s">
+        <v>99</v>
+      </c>
+      <c r="D168" t="s">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A169" t="s">
         <v>578</v>
       </c>
-      <c r="D161" t="s">
+      <c r="B169" t="s">
         <v>579</v>
       </c>
-    </row>
-    <row r="162" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A162" t="s">
+      <c r="C169" t="s">
         <v>580</v>
       </c>
-      <c r="B162" t="s">
+      <c r="D169" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A170" t="s">
         <v>581</v>
       </c>
-      <c r="C162" t="s">
+      <c r="B170" t="s">
         <v>582</v>
       </c>
-      <c r="D162" t="s">
+      <c r="C170" t="s">
         <v>583</v>
       </c>
-    </row>
-    <row r="163" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A163" t="s">
+      <c r="D170" t="s">
         <v>584</v>
       </c>
-      <c r="B163" t="s">
+    </row>
+    <row r="171" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A171" t="s">
         <v>585</v>
       </c>
-      <c r="C163" t="s">
+      <c r="B171" t="s">
         <v>586</v>
       </c>
-      <c r="D163" t="s">
+      <c r="C171" t="s">
         <v>587</v>
       </c>
-    </row>
-    <row r="164" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A164" t="s">
+      <c r="D171" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A172" t="s">
         <v>588</v>
       </c>
-      <c r="B164" t="s">
+      <c r="B172" t="s">
         <v>589</v>
       </c>
-      <c r="C164" t="s">
+      <c r="C172" t="s">
         <v>590</v>
       </c>
-      <c r="D164" t="s">
+      <c r="D172" t="s">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A173" t="s">
         <v>591</v>
       </c>
-    </row>
-    <row r="165" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A165" t="s">
+      <c r="B173" t="s">
         <v>592</v>
       </c>
-      <c r="B165" t="s">
+      <c r="C173" t="s">
         <v>593</v>
       </c>
-      <c r="C165" t="s">
+      <c r="D173" t="s">
         <v>594</v>
       </c>
-      <c r="D165" t="s">
+    </row>
+    <row r="174" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A174" t="s">
         <v>595</v>
       </c>
-    </row>
-    <row r="166" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A166" t="s">
+      <c r="B174" t="s">
         <v>596</v>
       </c>
-      <c r="B166" t="s">
+      <c r="C174" t="s">
         <v>597</v>
       </c>
-      <c r="C166" t="s">
+      <c r="D174" t="s">
         <v>598</v>
       </c>
-      <c r="D166" t="s">
+    </row>
+    <row r="175" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A175" t="s">
         <v>599</v>
       </c>
-    </row>
-    <row r="167" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A167" t="s">
+      <c r="B175" t="s">
         <v>600</v>
       </c>
-      <c r="B167" t="s">
+      <c r="C175" t="s">
         <v>601</v>
       </c>
-      <c r="C167" t="s">
+      <c r="D175" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A176" t="s">
         <v>602</v>
       </c>
-      <c r="D167" t="s">
+      <c r="B176" t="s">
+        <v>600</v>
+      </c>
+      <c r="C176" t="s">
         <v>603</v>
       </c>
-    </row>
-    <row r="168" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A168" t="s">
+      <c r="D176" t="s">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A177" t="s">
         <v>604</v>
       </c>
-      <c r="B168" t="s">
+      <c r="B177" t="s">
         <v>605</v>
       </c>
-      <c r="C168" t="s">
-        <v>102</v>
-      </c>
-      <c r="D168" t="s">
+      <c r="C177" t="s">
         <v>606</v>
       </c>
-    </row>
-    <row r="169" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A169" t="s">
+      <c r="D177" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A178" t="s">
         <v>607</v>
       </c>
-      <c r="B169" t="s">
+      <c r="B178" t="s">
         <v>608</v>
       </c>
-      <c r="C169" t="s">
+      <c r="C178" t="s">
         <v>609</v>
       </c>
-      <c r="D169" t="s">
+      <c r="D178" t="s">
         <v>610</v>
       </c>
     </row>
-    <row r="170" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A170" t="s">
+    <row r="179" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A179" t="s">
         <v>611</v>
       </c>
-      <c r="B170" t="s">
+      <c r="B179" t="s">
         <v>612</v>
       </c>
-      <c r="C170" t="s">
+      <c r="C179" t="s">
         <v>613</v>
       </c>
-      <c r="D170" t="s">
+      <c r="D179" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A180" t="s">
         <v>614</v>
       </c>
-    </row>
-    <row r="171" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A171" t="s">
+      <c r="B180" t="s">
         <v>615</v>
       </c>
-      <c r="B171" t="s">
+      <c r="C180" t="s">
         <v>616</v>
       </c>
-      <c r="C171" t="s">
+      <c r="D180" t="s">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A181" t="s">
         <v>617</v>
       </c>
-      <c r="D171" t="s">
+      <c r="B181" t="s">
+        <v>615</v>
+      </c>
+      <c r="C181" t="s">
         <v>618</v>
       </c>
-    </row>
-    <row r="172" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A172" t="s">
+      <c r="D181" t="s">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A182" t="s">
         <v>619</v>
       </c>
-      <c r="B172" t="s">
+      <c r="B182" t="s">
         <v>620</v>
       </c>
-      <c r="C172" t="s">
+      <c r="C182" t="s">
         <v>621</v>
       </c>
-      <c r="D172" t="s">
+      <c r="D182" t="s">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="183" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A183" t="s">
         <v>622</v>
       </c>
-    </row>
-    <row r="173" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A173" t="s">
+      <c r="B183" t="s">
         <v>623</v>
       </c>
-      <c r="B173" t="s">
+      <c r="C183" t="s">
         <v>624</v>
       </c>
-      <c r="C173" t="s">
+      <c r="D183" t="s">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A184" t="s">
         <v>625</v>
       </c>
-      <c r="D173" t="s">
+      <c r="B184" t="s">
         <v>626</v>
       </c>
-    </row>
-    <row r="174" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A174" t="s">
+      <c r="C184" t="s">
         <v>627</v>
       </c>
-      <c r="B174" t="s">
+      <c r="D184" t="s">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A185" t="s">
         <v>628</v>
       </c>
-      <c r="C174" t="s">
+      <c r="B185" t="s">
         <v>629</v>
       </c>
-      <c r="D174" t="s">
+      <c r="C185" t="s">
         <v>630</v>
       </c>
-    </row>
-    <row r="175" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A175" t="s">
+      <c r="D185" t="s">
         <v>631</v>
       </c>
-      <c r="B175" t="s">
+    </row>
+    <row r="186" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A186" t="s">
         <v>632</v>
       </c>
-      <c r="C175" t="s">
+      <c r="B186" t="s">
+        <v>629</v>
+      </c>
+      <c r="C186" t="s">
         <v>633</v>
       </c>
-      <c r="D175" t="s">
+      <c r="D186" t="s">
+        <v>676</v>
+      </c>
+    </row>
+    <row r="187" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A187" t="s">
         <v>634</v>
       </c>
-    </row>
-    <row r="176" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A176" t="s">
+      <c r="B187" t="s">
         <v>635</v>
       </c>
-      <c r="B176" t="s">
-        <v>632</v>
-      </c>
-      <c r="C176" t="s">
+      <c r="C187" t="s">
         <v>636</v>
-      </c>
-      <c r="D176" t="s">
-        <v>634</v>
-      </c>
-    </row>
-    <row r="177" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A177" t="s">
-        <v>637</v>
-      </c>
-      <c r="B177" t="s">
-        <v>638</v>
-      </c>
-      <c r="C177" t="s">
-        <v>639</v>
-      </c>
-      <c r="D177" t="s">
-        <v>640</v>
-      </c>
-    </row>
-    <row r="178" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A178" t="s">
-        <v>641</v>
-      </c>
-      <c r="B178" t="s">
-        <v>642</v>
-      </c>
-      <c r="C178" t="s">
-        <v>643</v>
-      </c>
-      <c r="D178" t="s">
-        <v>644</v>
-      </c>
-    </row>
-    <row r="179" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A179" t="s">
-        <v>645</v>
-      </c>
-      <c r="B179" t="s">
-        <v>646</v>
-      </c>
-      <c r="C179" t="s">
-        <v>647</v>
-      </c>
-      <c r="D179" t="s">
-        <v>648</v>
-      </c>
-    </row>
-    <row r="180" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A180" t="s">
-        <v>649</v>
-      </c>
-      <c r="B180" t="s">
-        <v>650</v>
-      </c>
-      <c r="C180" t="s">
-        <v>651</v>
-      </c>
-      <c r="D180" t="s">
-        <v>652</v>
-      </c>
-    </row>
-    <row r="181" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A181" t="s">
-        <v>653</v>
-      </c>
-      <c r="B181" t="s">
-        <v>650</v>
-      </c>
-      <c r="C181" t="s">
-        <v>654</v>
-      </c>
-      <c r="D181" t="s">
-        <v>652</v>
-      </c>
-    </row>
-    <row r="182" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A182" t="s">
-        <v>655</v>
-      </c>
-      <c r="B182" t="s">
-        <v>656</v>
-      </c>
-      <c r="C182" t="s">
-        <v>657</v>
-      </c>
-      <c r="D182" t="s">
-        <v>658</v>
-      </c>
-    </row>
-    <row r="183" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A183" t="s">
-        <v>659</v>
-      </c>
-      <c r="B183" t="s">
-        <v>660</v>
-      </c>
-      <c r="C183" t="s">
-        <v>661</v>
-      </c>
-      <c r="D183" t="s">
-        <v>662</v>
-      </c>
-    </row>
-    <row r="184" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A184" t="s">
-        <v>663</v>
-      </c>
-      <c r="B184" t="s">
-        <v>664</v>
-      </c>
-      <c r="C184" t="s">
-        <v>665</v>
-      </c>
-      <c r="D184" t="s">
-        <v>666</v>
-      </c>
-    </row>
-    <row r="185" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A185" t="s">
-        <v>667</v>
-      </c>
-      <c r="B185" t="s">
-        <v>668</v>
-      </c>
-      <c r="C185" t="s">
-        <v>669</v>
-      </c>
-      <c r="D185" t="s">
-        <v>670</v>
-      </c>
-    </row>
-    <row r="186" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A186" t="s">
-        <v>671</v>
-      </c>
-      <c r="B186" t="s">
-        <v>668</v>
-      </c>
-      <c r="C186" t="s">
-        <v>672</v>
-      </c>
-      <c r="D186" t="s">
-        <v>673</v>
-      </c>
-    </row>
-    <row r="187" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A187" t="s">
-        <v>674</v>
-      </c>
-      <c r="B187" t="s">
-        <v>675</v>
-      </c>
-      <c r="C187" t="s">
-        <v>676</v>
       </c>
       <c r="D187" t="s">
         <v>677</v>
       </c>
     </row>
-    <row r="188" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
+        <v>637</v>
+      </c>
+      <c r="B188" t="s">
+        <v>638</v>
+      </c>
+      <c r="C188" t="s">
+        <v>639</v>
+      </c>
+      <c r="D188" t="s">
         <v>678</v>
       </c>
-      <c r="B188" t="s">
+    </row>
+    <row r="189" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A189" t="s">
+        <v>640</v>
+      </c>
+      <c r="B189" t="s">
+        <v>641</v>
+      </c>
+      <c r="C189" t="s">
+        <v>642</v>
+      </c>
+      <c r="D189" t="s">
         <v>679</v>
       </c>
-      <c r="C188" t="s">
-        <v>680</v>
-      </c>
-      <c r="D188" t="s">
-        <v>681</v>
-      </c>
-    </row>
-    <row r="189" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A189" t="s">
-        <v>682</v>
-      </c>
-      <c r="B189" t="s">
-        <v>683</v>
-      </c>
-      <c r="C189" t="s">
-        <v>684</v>
-      </c>
-      <c r="D189" t="s">
-        <v>685</v>
-      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
testing and database improvements
</commit_message>
<xml_diff>
--- a/backend/api/servicehandler/services/ABA IBI Providers.xlsx
+++ b/backend/api/servicehandler/services/ABA IBI Providers.xlsx
@@ -1,27 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://utoronto-my.sharepoint.com/personal/behnaz_merikhi_utoronto_ca/Documents/ASD Project/DB/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dextertam/Documents/UofT/Y3/_Extracurricular/AutismCanadaAI/backend/api/servicehandler/services/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{3F7D9D29-FF0B-46FB-975F-D4C7ADA165B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{343F658E-99B6-7545-AAA9-2A6C7CCB7BD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="-28300" windowWidth="51200" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Recovered_Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="756" uniqueCount="690">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="755" uniqueCount="684">
   <si>
     <t>https://www.myautismguide.ca/mag/content/provider/1-step-ahead-services-inc?nid=561321</t>
   </si>
@@ -56,9 +55,6 @@
     <t>ON</t>
   </si>
   <si>
-    <t>519-257-8259</t>
-  </si>
-  <si>
     <t>https://www.myautismguide.ca/mag/content/provider/block-above-behavioral-consulting?nid=561331</t>
   </si>
   <si>
@@ -236,9 +232,6 @@
     <t>335 Habkirk Dr Regina, SKS4S 6A9</t>
   </si>
   <si>
-    <t>306-570-4273</t>
-  </si>
-  <si>
     <t>https://www.myautismguide.ca/mag/content/provider/above-and-beyond-autism-consulting-services?nid=581146</t>
   </si>
   <si>
@@ -293,9 +286,6 @@
     <t>36 antares Drive Ottawa, ONK2E 7W5</t>
   </si>
   <si>
-    <t>343-887-2287</t>
-  </si>
-  <si>
     <t>https://www.myautismguide.ca/mag/content/provider/aim-pediatric-therapy-2?nid=569731</t>
   </si>
   <si>
@@ -377,9 +367,6 @@
     <t>36-5200 Dallas Drive Kamloops, BCV2C 6Y8</t>
   </si>
   <si>
-    <t>250-299-3530</t>
-  </si>
-  <si>
     <t>https://www.myautismguide.ca/mag/content/provider/applied-behavioural-interventions?nid=569861</t>
   </si>
   <si>
@@ -437,9 +424,6 @@
     <t>2006 Robertson rd Ottawa, ON</t>
   </si>
   <si>
-    <t>(613) 680-4700          (613) 424-0442</t>
-  </si>
-  <si>
     <t>https://www.myautismguide.ca/mag/content/provider/aspiration-discoveries?nid=569916</t>
   </si>
   <si>
@@ -776,9 +760,6 @@
     <t>L3 30 Dupont Street East Waterloo, ONN2J 2G9</t>
   </si>
   <si>
-    <t>226-755-0015</t>
-  </si>
-  <si>
     <t>https://www.myautismguide.ca/mag/content/provider/beyond-services-choice-matters?nid=570386</t>
   </si>
   <si>
@@ -812,9 +793,6 @@
     <t>5836 Leslie Street Suite 809 Toronto, ONM2H 1J8</t>
   </si>
   <si>
-    <t>416-554-8716</t>
-  </si>
-  <si>
     <t>https://www.myautismguide.ca/mag/content/provider/beyond-spectrum?nid=570396</t>
   </si>
   <si>
@@ -872,9 +850,6 @@
     <t>85 Le Maire St. Winnipeg, MBR3V 1E1</t>
   </si>
   <si>
-    <t>431-531-8701</t>
-  </si>
-  <si>
     <t>https://www.myautismguide.ca/mag/content/provider/blue-lantern-learning?nid=566766</t>
   </si>
   <si>
@@ -1094,9 +1069,6 @@
     <t>3rd Floor, WMRH P.O Box 2005 Corner Brooke, NLA2H 6J7</t>
   </si>
   <si>
-    <t>7096375000 6655</t>
-  </si>
-  <si>
     <t>https://www.myautismguide.ca/mag/content/provider/childrens-development-group?nid=571431</t>
   </si>
   <si>
@@ -1202,9 +1174,6 @@
     <t>Markham, ON</t>
   </si>
   <si>
-    <t>416-993-4369</t>
-  </si>
-  <si>
     <t>https://www.myautismguide.ca/mag/content/provider/dr-kiran-pure-associates?nid=568496</t>
   </si>
   <si>
@@ -1307,9 +1276,6 @@
     <t>10145 McVean Drive   Brampton,, ONL6P 4K7</t>
   </si>
   <si>
-    <t>1-877-374-6625</t>
-  </si>
-  <si>
     <t>https://www.myautismguide.ca/mag/content/provider/erinoakkids-centre-treatment-and-development-0?nid=585846</t>
   </si>
   <si>
@@ -1337,9 +1303,6 @@
     <t>520 Westney Road S Ajax, ONL1S 6W4</t>
   </si>
   <si>
-    <t>1(866) 211-7779</t>
-  </si>
-  <si>
     <t>https://www.myautismguide.ca/mag/content/provider/exceptional-minds?nid=572641</t>
   </si>
   <si>
@@ -1385,9 +1348,6 @@
     <t>5703, rue Ferrier Mont-Royal, QCH4P 1N3</t>
   </si>
   <si>
-    <t>514.345.1300</t>
-  </si>
-  <si>
     <t>https://www.myautismguide.ca/mag/content/provider/functional-learning-centre?nid=563176</t>
   </si>
   <si>
@@ -1511,9 +1471,6 @@
     <t>14487 78th Avenue  Surrey, BCV3S 9C5</t>
   </si>
   <si>
-    <t>604-572-1126</t>
-  </si>
-  <si>
     <t>https://www.myautismguide.ca/mag/content/provider/helping-hands-behaviour-consulting?nid=563381</t>
   </si>
   <si>
@@ -1556,9 +1513,6 @@
     <t>231 Elm Beaconsfield, QCH9W 2E2</t>
   </si>
   <si>
-    <t>5146953914#3304</t>
-  </si>
-  <si>
     <t>https://www.myautismguide.ca/mag/content/provider/i-believe-miracles?nid=573331</t>
   </si>
   <si>
@@ -1643,9 +1597,6 @@
     <t>Durham Region, ON</t>
   </si>
   <si>
-    <t>905-914-0405</t>
-  </si>
-  <si>
     <t>https://www.myautismguide.ca/mag/content/provider/jhmj-coaching-consulting?nid=562846</t>
   </si>
   <si>
@@ -1655,9 +1606,6 @@
     <t>BC</t>
   </si>
   <si>
-    <t>250-597-8997</t>
-  </si>
-  <si>
     <t>https://www.myautismguide.ca/mag/content/provider/joy-behaviour-consulting-intervention?nid=559841</t>
   </si>
   <si>
@@ -1697,9 +1645,6 @@
     <t>Ottawa, ON</t>
   </si>
   <si>
-    <t>613-327-5775</t>
-  </si>
-  <si>
     <t>https://www.myautismguide.ca/mag/content/provider/mcmaster-autism-program?nid=601316</t>
   </si>
   <si>
@@ -1709,9 +1654,6 @@
     <t>325 Wellington St N Hamilton , ONM5V 1E7</t>
   </si>
   <si>
-    <t>905-521-2100</t>
-  </si>
-  <si>
     <t>https://www.myautismguide.ca/mag/content/provider/moving-forward-autism-services-tools-inc?nid=588541</t>
   </si>
   <si>
@@ -1721,9 +1663,6 @@
     <t>1200 Lawrence Ave East Suite 304 North York, ONM3A 1C1</t>
   </si>
   <si>
-    <t>647-468-0474</t>
-  </si>
-  <si>
     <t>https://www.myautismguide.ca/mag/content/provider/nunavummi-disabilities-makinnasuaqtiit-society?nid=588576</t>
   </si>
   <si>
@@ -1733,9 +1672,6 @@
     <t>PO Box 4212 Iqaluit, NUX0A1H0</t>
   </si>
   <si>
-    <t>867-979-2228</t>
-  </si>
-  <si>
     <t>https://www.myautismguide.ca/mag/content/provider/oap-provider-list?nid=593141</t>
   </si>
   <si>
@@ -1751,18 +1687,12 @@
     <t>32 Elgin St. East Oshawa, ONL1G1T1</t>
   </si>
   <si>
-    <t>4164549340</t>
-  </si>
-  <si>
     <t>https://www.myautismguide.ca/mag/content/provider/one-care-inc-0?nid=588586</t>
   </si>
   <si>
     <t>169-173 Simcoe St. North Oshawa, ONL1G 4S8</t>
   </si>
   <si>
-    <t>905 2402203</t>
-  </si>
-  <si>
     <t>https://www.myautismguide.ca/mag/content/provider/osns-child-youth-development-centre?nid=564966</t>
   </si>
   <si>
@@ -1784,9 +1714,6 @@
     <t>12-52 Antares Ottawa, ONK2E 7Z1</t>
   </si>
   <si>
-    <t>(613)212-4828</t>
-  </si>
-  <si>
     <t>https://www.myautismguide.ca/mag/content/provider/parley-services-limited?nid=588611</t>
   </si>
   <si>
@@ -1796,9 +1723,6 @@
     <t>Suite 1703, 805 West Broadway Vancouver, BCV5Z 1K1</t>
   </si>
   <si>
-    <t>604-868-5586</t>
-  </si>
-  <si>
     <t>https://www.myautismguide.ca/mag/content/provider/pivot-point-family-growth-centre-inc-11?nid=588626</t>
   </si>
   <si>
@@ -1808,9 +1732,6 @@
     <t>#24 15515 24th Avenue Surrey, BCV4A 2J4</t>
   </si>
   <si>
-    <t>604.531.4544</t>
-  </si>
-  <si>
     <t>https://www.myautismguide.ca/mag/content/provider/positive-behavioral-supports-corp-canada?nid=588631</t>
   </si>
   <si>
@@ -1820,9 +1741,6 @@
     <t>99 Oswell Dr. Ajax, ONL1Z 0L5</t>
   </si>
   <si>
-    <t>6473602700 X 1163</t>
-  </si>
-  <si>
     <t>https://www.myautismguide.ca/mag/content/provider/precious-souls-services-inc?nid=588636</t>
   </si>
   <si>
@@ -1832,18 +1750,12 @@
     <t>7330 Goreway Drive Mississauga, ONL4T 4J2</t>
   </si>
   <si>
-    <t>647-948-8080</t>
-  </si>
-  <si>
     <t>https://www.myautismguide.ca/mag/content/provider/santana-behavioural-services?nid=588681</t>
   </si>
   <si>
     <t>Santana Behavioural Services</t>
   </si>
   <si>
-    <t>647-588-0271</t>
-  </si>
-  <si>
     <t>https://www.myautismguide.ca/mag/content/provider/shining-through-centre-2?nid=588701</t>
   </si>
   <si>
@@ -1853,9 +1765,6 @@
     <t>7365 Martin Grove Rd Woodbridge, ONL4L 9E4</t>
   </si>
   <si>
-    <t>905-851-7955</t>
-  </si>
-  <si>
     <t>https://www.myautismguide.ca/mag/content/provider/south-asian-autism-awareness-center?nid=577136</t>
   </si>
   <si>
@@ -1877,9 +1786,6 @@
     <t>489c Tennyson Place Victoria, BCV8Z 3P6</t>
   </si>
   <si>
-    <t>250-472-8304</t>
-  </si>
-  <si>
     <t>https://www.myautismguide.ca/mag/content/provider/success-steps-0?nid=588766</t>
   </si>
   <si>
@@ -1889,9 +1795,6 @@
     <t>13 Dallas Place Ottawa, ONK2G 3E2</t>
   </si>
   <si>
-    <t>613-882-7688</t>
-  </si>
-  <si>
     <t>https://www.myautismguide.ca/mag/content/provider/sue-larke?nid=560121</t>
   </si>
   <si>
@@ -1925,9 +1828,6 @@
     <t>547 Upper James Street Hamilton, ONL9C 2Y5</t>
   </si>
   <si>
-    <t>289-755-7891</t>
-  </si>
-  <si>
     <t>https://www.myautismguide.ca/mag/content/provider/teach-me-my-way-services-0?nid=597546</t>
   </si>
   <si>
@@ -1943,9 +1843,6 @@
     <t>685 Kennedy Road #5 Scarborough , ONM1K 2B8</t>
   </si>
   <si>
-    <t>647-330-6130</t>
-  </si>
-  <si>
     <t>https://www.myautismguide.ca/mag/content/provider/birch-centre-learning-and-development-aba-therapy?nid=595071</t>
   </si>
   <si>
@@ -1967,9 +1864,6 @@
     <t>63 Fernbank Place  Whitby, ONL1R 1T1</t>
   </si>
   <si>
-    <t>905 626 0377</t>
-  </si>
-  <si>
     <t>https://www.myautismguide.ca/mag/content/provider/toronto-ibi-0?nid=588811</t>
   </si>
   <si>
@@ -1979,9 +1873,6 @@
     <t>32-1170 Sheppard Ave. W North York, ONM3K 2A3</t>
   </si>
   <si>
-    <t>416-614-9025</t>
-  </si>
-  <si>
     <t>https://www.myautismguide.ca/mag/content/provider/toronto-ibi-1?nid=588816</t>
   </si>
   <si>
@@ -1997,9 +1888,6 @@
     <t>Suite 112/210 2800 High Point Drive Milton, ONL9T 6P4</t>
   </si>
   <si>
-    <t>365 877 9094</t>
-  </si>
-  <si>
     <t>https://www.myautismguide.ca/mag/content/provider/valley-child-development-association-0?nid=588841</t>
   </si>
   <si>
@@ -2009,9 +1897,6 @@
     <t>28 Aberdeen St, Suite 5 Kentville, NSB4N 2N1</t>
   </si>
   <si>
-    <t>902-678-6111</t>
-  </si>
-  <si>
     <t>https://www.myautismguide.ca/mag/content/provider/wes-consortium?nid=589301</t>
   </si>
   <si>
@@ -2021,9 +1906,6 @@
     <t>Brampton, ON</t>
   </si>
   <si>
-    <t>905-439-9280</t>
-  </si>
-  <si>
     <t>https://www.myautismguide.ca/mag/content/provider/wirth-behavioural-health-services?nid=567201</t>
   </si>
   <si>
@@ -2042,9 +1924,6 @@
     <t>32 Woodstone Dr East St. Paul, MBR2E 0M5</t>
   </si>
   <si>
-    <t>204-807-6779</t>
-  </si>
-  <si>
     <t>https://www.myautismguide.ca/mag/content/provider/woodview-mental-health-autism-services?nid=578426</t>
   </si>
   <si>
@@ -2054,9 +1933,6 @@
     <t>50 Fairwood Place W Burlington, ONL7T 1E5</t>
   </si>
   <si>
-    <t>905 689 4727</t>
-  </si>
-  <si>
     <t>https://www.myautismguide.ca/mag/content/provider/woodview-mental-health-and-autism-services?nid=578486</t>
   </si>
   <si>
@@ -2066,9 +1942,6 @@
     <t>643 Park Road North Brantford, ONN3T 5L8</t>
   </si>
   <si>
-    <t>519 752 5308</t>
-  </si>
-  <si>
     <t>https://www.myautismguide.ca/mag/content/provider/york-autism-centre-making-small-talk?nid=588901</t>
   </si>
   <si>
@@ -2078,9 +1951,6 @@
     <t>73 Industrial Parkway North - Unit 4 Aurora, ONL4C 4C4</t>
   </si>
   <si>
-    <t>647-519-6739</t>
-  </si>
-  <si>
     <t>Organization</t>
   </si>
   <si>
@@ -2091,13 +1961,124 @@
   </si>
   <si>
     <t>Phone</t>
+  </si>
+  <si>
+    <t>(519) 257-8259</t>
+  </si>
+  <si>
+    <t>(343) 887-2287</t>
+  </si>
+  <si>
+    <t>(431) 531-8701</t>
+  </si>
+  <si>
+    <t>(877) 374-6625</t>
+  </si>
+  <si>
+    <t>(866) 211-7779</t>
+  </si>
+  <si>
+    <t>(514) 345-1300</t>
+  </si>
+  <si>
+    <t>(905) 914-0405</t>
+  </si>
+  <si>
+    <t>(250) 597-8997</t>
+  </si>
+  <si>
+    <t>(613) 327-5775</t>
+  </si>
+  <si>
+    <t>(905) 521-2100</t>
+  </si>
+  <si>
+    <t>(647) 468-0474</t>
+  </si>
+  <si>
+    <t>(867) 979-2228</t>
+  </si>
+  <si>
+    <t>(416) 454-9340</t>
+  </si>
+  <si>
+    <t>(905) 240-2203</t>
+  </si>
+  <si>
+    <t>(604) 868-5586</t>
+  </si>
+  <si>
+    <t>(604) 531-4544</t>
+  </si>
+  <si>
+    <t>(647) 948-8080</t>
+  </si>
+  <si>
+    <t>(647) 588-0271</t>
+  </si>
+  <si>
+    <t>(905) 851-7955</t>
+  </si>
+  <si>
+    <t>(250) 472-8304</t>
+  </si>
+  <si>
+    <t>(613) 882-7688</t>
+  </si>
+  <si>
+    <t>(289) 755-7891</t>
+  </si>
+  <si>
+    <t>(289) 755-7892</t>
+  </si>
+  <si>
+    <t>(647) 330-6130</t>
+  </si>
+  <si>
+    <t>(905) 626-0377</t>
+  </si>
+  <si>
+    <t>(416) 614-9025</t>
+  </si>
+  <si>
+    <t>(365) 877-9094</t>
+  </si>
+  <si>
+    <t>(902) 678-6111</t>
+  </si>
+  <si>
+    <t>(905) 439-9280</t>
+  </si>
+  <si>
+    <t>(204) 807-6780</t>
+  </si>
+  <si>
+    <t>(905) 689-4727</t>
+  </si>
+  <si>
+    <t>(519) 752-5308</t>
+  </si>
+  <si>
+    <t>(647) 519-6739</t>
+  </si>
+  <si>
+    <t>(613) 680-4700</t>
+  </si>
+  <si>
+    <t>(613) 212-4828</t>
+  </si>
+  <si>
+    <t>(514) 695-3914</t>
+  </si>
+  <si>
+    <t>(709) 637-5000 6655</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2109,6 +2090,12 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -2478,33 +2465,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D189"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+    <sheetView tabSelected="1" zoomScale="132" workbookViewId="0">
+      <selection activeCell="F92" sqref="F92"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="53.625" customWidth="1"/>
-    <col min="2" max="2" width="35.25" customWidth="1"/>
-    <col min="3" max="3" width="39.875" customWidth="1"/>
-    <col min="4" max="4" width="31.625" customWidth="1"/>
+    <col min="1" max="1" width="93" customWidth="1"/>
+    <col min="2" max="2" width="60.6640625" customWidth="1"/>
+    <col min="3" max="3" width="35.33203125" customWidth="1"/>
+    <col min="4" max="4" width="31.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>687</v>
+        <v>644</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>686</v>
+        <v>643</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>688</v>
+        <v>645</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>689</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2518,7 +2505,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -2532,7 +2519,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -2543,2600 +2530,2598 @@
         <v>10</v>
       </c>
       <c r="D4" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="B5" t="s">
         <v>12</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>13</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>14</v>
       </c>
-      <c r="D5" t="s">
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="B6" t="s">
         <v>16</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>17</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>18</v>
       </c>
-      <c r="D6" t="s">
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="B7" t="s">
         <v>20</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>21</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>22</v>
       </c>
-      <c r="D7" t="s">
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="B8" t="s">
         <v>24</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>25</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>26</v>
       </c>
-      <c r="D8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="B9" t="s">
         <v>27</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>28</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>29</v>
       </c>
-      <c r="D9" t="s">
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="B10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" t="s">
         <v>31</v>
       </c>
-      <c r="B10" t="s">
-        <v>28</v>
-      </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>32</v>
       </c>
-      <c r="D10" t="s">
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="B11" t="s">
         <v>34</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>35</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>36</v>
       </c>
-      <c r="D11" t="s">
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="B12" t="s">
         <v>38</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>39</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>40</v>
       </c>
-      <c r="D12" t="s">
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="B13" t="s">
         <v>42</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>43</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>44</v>
       </c>
-      <c r="D13" t="s">
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="B14" t="s">
         <v>46</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>47</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>48</v>
       </c>
-      <c r="D14" t="s">
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="B15" t="s">
         <v>50</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>51</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>52</v>
       </c>
-      <c r="D15" t="s">
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="B16" t="s">
         <v>54</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>55</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>56</v>
       </c>
-      <c r="D16" t="s">
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="B17" t="s">
         <v>58</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>59</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>60</v>
       </c>
-      <c r="D17" t="s">
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="B18" t="s">
+        <v>58</v>
+      </c>
+      <c r="C18" t="s">
         <v>62</v>
       </c>
-      <c r="B18" t="s">
-        <v>59</v>
-      </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>63</v>
       </c>
-      <c r="D18" t="s">
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="B19" t="s">
+        <v>58</v>
+      </c>
+      <c r="C19" t="s">
         <v>65</v>
       </c>
-      <c r="B19" t="s">
-        <v>59</v>
-      </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>66</v>
       </c>
-      <c r="D19" t="s">
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="B20" t="s">
         <v>68</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>69</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
         <v>70</v>
       </c>
-      <c r="D20" t="s">
+      <c r="B21" t="s">
+        <v>68</v>
+      </c>
+      <c r="C21" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="D21" t="s">
         <v>72</v>
       </c>
-      <c r="B21" t="s">
-        <v>69</v>
-      </c>
-      <c r="C21" t="s">
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
         <v>73</v>
       </c>
-      <c r="D21" t="s">
+      <c r="B22" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="C22" t="s">
         <v>75</v>
       </c>
-      <c r="B22" t="s">
+      <c r="D22" t="s">
         <v>76</v>
       </c>
-      <c r="C22" t="s">
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
         <v>77</v>
       </c>
-      <c r="D22" t="s">
+      <c r="B23" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="C23" t="s">
         <v>79</v>
       </c>
-      <c r="B23" t="s">
+      <c r="D23" t="s">
         <v>80</v>
       </c>
-      <c r="C23" t="s">
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
         <v>81</v>
       </c>
-      <c r="D23" t="s">
+      <c r="B24" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="C24" t="s">
         <v>83</v>
       </c>
-      <c r="B24" t="s">
+      <c r="D24" t="s">
         <v>84</v>
       </c>
-      <c r="C24" t="s">
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
         <v>85</v>
       </c>
-      <c r="D24" t="s">
+      <c r="B25" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="C25" t="s">
         <v>87</v>
       </c>
-      <c r="B25" t="s">
+      <c r="D25" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
         <v>88</v>
       </c>
-      <c r="C25" t="s">
+      <c r="B26" t="s">
         <v>89</v>
       </c>
-      <c r="D25" t="s">
+      <c r="C26" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="D26" t="s">
         <v>91</v>
       </c>
-      <c r="B26" t="s">
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
         <v>92</v>
       </c>
-      <c r="C26" t="s">
+      <c r="B27" t="s">
+        <v>89</v>
+      </c>
+      <c r="C27" t="s">
         <v>93</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D27" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="B28" t="s">
+        <v>89</v>
+      </c>
+      <c r="C28" t="s">
         <v>95</v>
       </c>
-      <c r="B27" t="s">
-        <v>92</v>
-      </c>
-      <c r="C27" t="s">
+      <c r="D28" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
         <v>96</v>
       </c>
-      <c r="D27" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="B29" t="s">
+        <v>89</v>
+      </c>
+      <c r="C29" t="s">
         <v>97</v>
       </c>
-      <c r="B28" t="s">
-        <v>92</v>
-      </c>
-      <c r="C28" t="s">
+      <c r="D29" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
         <v>98</v>
       </c>
-      <c r="D28" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="B30" t="s">
+        <v>89</v>
+      </c>
+      <c r="C30" t="s">
         <v>99</v>
       </c>
-      <c r="B29" t="s">
-        <v>92</v>
-      </c>
-      <c r="C29" t="s">
+      <c r="D30" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
         <v>100</v>
       </c>
-      <c r="D29" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+      <c r="B31" t="s">
+        <v>89</v>
+      </c>
+      <c r="C31" t="s">
         <v>101</v>
       </c>
-      <c r="B30" t="s">
-        <v>92</v>
-      </c>
-      <c r="C30" t="s">
+      <c r="D31" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
         <v>102</v>
       </c>
-      <c r="D30" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+      <c r="B32" t="s">
+        <v>89</v>
+      </c>
+      <c r="C32" t="s">
         <v>103</v>
       </c>
-      <c r="B31" t="s">
-        <v>92</v>
-      </c>
-      <c r="C31" t="s">
+      <c r="D32" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
         <v>104</v>
       </c>
-      <c r="D31" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+      <c r="B33" t="s">
         <v>105</v>
       </c>
-      <c r="B32" t="s">
-        <v>92</v>
-      </c>
-      <c r="C32" t="s">
+      <c r="C33" t="s">
         <v>106</v>
       </c>
-      <c r="D32" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+      <c r="D33" t="s">
         <v>107</v>
       </c>
-      <c r="B33" t="s">
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
         <v>108</v>
       </c>
-      <c r="C33" t="s">
+      <c r="B34" t="s">
         <v>109</v>
       </c>
-      <c r="D33" t="s">
+      <c r="C34" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+      <c r="D34" t="s">
         <v>111</v>
       </c>
-      <c r="B34" t="s">
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
         <v>112</v>
       </c>
-      <c r="C34" t="s">
+      <c r="B35" t="s">
         <v>113</v>
       </c>
-      <c r="D34" t="s">
+      <c r="C35" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+      <c r="D35" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
         <v>115</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B36" t="s">
         <v>116</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C36" t="s">
         <v>117</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D36" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
         <v>119</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B37" t="s">
         <v>120</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C37" t="s">
         <v>121</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D37" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
         <v>123</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B38" t="s">
         <v>124</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C38" t="s">
         <v>125</v>
       </c>
-      <c r="D37" t="s">
+      <c r="D38" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
         <v>127</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B39" t="s">
         <v>128</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C39" t="s">
         <v>129</v>
       </c>
-      <c r="D38" t="s">
+      <c r="D39" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
         <v>131</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B40" t="s">
         <v>132</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C40" t="s">
         <v>133</v>
       </c>
-      <c r="D39" t="s">
+      <c r="D40" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+      <c r="B41" t="s">
         <v>135</v>
       </c>
-      <c r="B40" t="s">
+      <c r="C41" t="s">
         <v>136</v>
       </c>
-      <c r="C40" t="s">
+      <c r="D41" t="s">
         <v>137</v>
       </c>
-      <c r="D40" t="s">
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+      <c r="B42" t="s">
         <v>139</v>
       </c>
-      <c r="B41" t="s">
+      <c r="C42" t="s">
         <v>140</v>
       </c>
-      <c r="C41" t="s">
+      <c r="D42" t="s">
         <v>141</v>
       </c>
-      <c r="D41" t="s">
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+      <c r="B43" t="s">
         <v>143</v>
       </c>
-      <c r="B42" t="s">
+      <c r="C43" t="s">
         <v>144</v>
       </c>
-      <c r="C42" t="s">
+      <c r="D43" t="s">
         <v>145</v>
       </c>
-      <c r="D42" t="s">
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+      <c r="B44" t="s">
         <v>147</v>
       </c>
-      <c r="B43" t="s">
+      <c r="C44" t="s">
         <v>148</v>
       </c>
-      <c r="C43" t="s">
+      <c r="D44" t="s">
         <v>149</v>
       </c>
-      <c r="D43" t="s">
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+      <c r="B45" t="s">
         <v>151</v>
       </c>
-      <c r="B44" t="s">
+      <c r="C45" t="s">
         <v>152</v>
       </c>
-      <c r="C44" t="s">
+      <c r="D45" t="s">
         <v>153</v>
       </c>
-      <c r="D44" t="s">
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+      <c r="B46" t="s">
         <v>155</v>
       </c>
-      <c r="B45" t="s">
+      <c r="C46" t="s">
         <v>156</v>
       </c>
-      <c r="C45" t="s">
+      <c r="D46" t="s">
         <v>157</v>
       </c>
-      <c r="D45" t="s">
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+      <c r="B47" t="s">
         <v>159</v>
       </c>
-      <c r="B46" t="s">
+      <c r="C47" t="s">
         <v>160</v>
       </c>
-      <c r="C46" t="s">
+      <c r="D47" t="s">
         <v>161</v>
       </c>
-      <c r="D46" t="s">
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+      <c r="B48" t="s">
         <v>163</v>
       </c>
-      <c r="B47" t="s">
+      <c r="C48" t="s">
         <v>164</v>
       </c>
-      <c r="C47" t="s">
+      <c r="D48" t="s">
         <v>165</v>
       </c>
-      <c r="D47" t="s">
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
+      <c r="B49" t="s">
         <v>167</v>
       </c>
-      <c r="B48" t="s">
+      <c r="C49" t="s">
         <v>168</v>
       </c>
-      <c r="C48" t="s">
+      <c r="D49" t="s">
         <v>169</v>
       </c>
-      <c r="D48" t="s">
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
+      <c r="B50" t="s">
+        <v>167</v>
+      </c>
+      <c r="C50" t="s">
         <v>171</v>
       </c>
-      <c r="B49" t="s">
+      <c r="D50" t="s">
         <v>172</v>
       </c>
-      <c r="C49" t="s">
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
         <v>173</v>
       </c>
-      <c r="D49" t="s">
+      <c r="B51" t="s">
+        <v>167</v>
+      </c>
+      <c r="C51" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
+      <c r="D51" t="s">
         <v>175</v>
       </c>
-      <c r="B50" t="s">
-        <v>172</v>
-      </c>
-      <c r="C50" t="s">
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
         <v>176</v>
       </c>
-      <c r="D50" t="s">
+      <c r="B52" t="s">
+        <v>167</v>
+      </c>
+      <c r="C52" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
+      <c r="D52" t="s">
         <v>178</v>
       </c>
-      <c r="B51" t="s">
-        <v>172</v>
-      </c>
-      <c r="C51" t="s">
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
         <v>179</v>
       </c>
-      <c r="D51" t="s">
+      <c r="B53" t="s">
+        <v>167</v>
+      </c>
+      <c r="C53" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
+      <c r="D53" t="s">
         <v>181</v>
       </c>
-      <c r="B52" t="s">
-        <v>172</v>
-      </c>
-      <c r="C52" t="s">
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
         <v>182</v>
       </c>
-      <c r="D52" t="s">
+      <c r="B54" t="s">
+        <v>167</v>
+      </c>
+      <c r="C54" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
+      <c r="D54" t="s">
         <v>184</v>
       </c>
-      <c r="B53" t="s">
-        <v>172</v>
-      </c>
-      <c r="C53" t="s">
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
         <v>185</v>
       </c>
-      <c r="D53" t="s">
+      <c r="B55" t="s">
+        <v>167</v>
+      </c>
+      <c r="C55" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
+      <c r="D55" t="s">
         <v>187</v>
       </c>
-      <c r="B54" t="s">
-        <v>172</v>
-      </c>
-      <c r="C54" t="s">
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
         <v>188</v>
       </c>
-      <c r="D54" t="s">
+      <c r="B56" t="s">
+        <v>167</v>
+      </c>
+      <c r="C56" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
+      <c r="D56" t="s">
         <v>190</v>
       </c>
-      <c r="B55" t="s">
-        <v>172</v>
-      </c>
-      <c r="C55" t="s">
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
         <v>191</v>
       </c>
-      <c r="D55" t="s">
+      <c r="B57" t="s">
+        <v>167</v>
+      </c>
+      <c r="C57" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
+      <c r="D57" t="s">
         <v>193</v>
       </c>
-      <c r="B56" t="s">
-        <v>172</v>
-      </c>
-      <c r="C56" t="s">
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
         <v>194</v>
       </c>
-      <c r="D56" t="s">
+      <c r="B58" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
+      <c r="C58" t="s">
         <v>196</v>
       </c>
-      <c r="B57" t="s">
-        <v>172</v>
-      </c>
-      <c r="C57" t="s">
+      <c r="D58" t="s">
         <v>197</v>
       </c>
-      <c r="D57" t="s">
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
+      <c r="B59" t="s">
         <v>199</v>
       </c>
-      <c r="B58" t="s">
+      <c r="C59" t="s">
         <v>200</v>
       </c>
-      <c r="C58" t="s">
+      <c r="D59" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
         <v>201</v>
       </c>
-      <c r="D58" t="s">
+      <c r="B60" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
+      <c r="C60" t="s">
         <v>203</v>
       </c>
-      <c r="B59" t="s">
+      <c r="D60" t="s">
         <v>204</v>
       </c>
-      <c r="C59" t="s">
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
         <v>205</v>
       </c>
-      <c r="D59" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
+      <c r="B61" t="s">
         <v>206</v>
       </c>
-      <c r="B60" t="s">
+      <c r="C61" t="s">
         <v>207</v>
       </c>
-      <c r="C60" t="s">
+      <c r="D61" t="s">
         <v>208</v>
       </c>
-      <c r="D60" t="s">
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
+      <c r="B62" t="s">
         <v>210</v>
       </c>
-      <c r="B61" t="s">
+      <c r="C62" t="s">
         <v>211</v>
       </c>
-      <c r="C61" t="s">
+      <c r="D62" t="s">
         <v>212</v>
       </c>
-      <c r="D61" t="s">
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
+      <c r="B63" t="s">
         <v>214</v>
       </c>
-      <c r="B62" t="s">
+      <c r="C63" t="s">
         <v>215</v>
       </c>
-      <c r="C62" t="s">
+      <c r="D63" t="s">
         <v>216</v>
       </c>
-      <c r="D62" t="s">
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
+      <c r="B64" t="s">
+        <v>214</v>
+      </c>
+      <c r="C64" t="s">
         <v>218</v>
       </c>
-      <c r="B63" t="s">
+      <c r="D64" t="s">
         <v>219</v>
       </c>
-      <c r="C63" t="s">
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
         <v>220</v>
       </c>
-      <c r="D63" t="s">
+      <c r="B65" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
+      <c r="C65" t="s">
         <v>222</v>
       </c>
-      <c r="B64" t="s">
-        <v>219</v>
-      </c>
-      <c r="C64" t="s">
+      <c r="D65" t="s">
         <v>223</v>
       </c>
-      <c r="D64" t="s">
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
+      <c r="B66" t="s">
+        <v>221</v>
+      </c>
+      <c r="C66" t="s">
         <v>225</v>
       </c>
-      <c r="B65" t="s">
+      <c r="D66" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
         <v>226</v>
       </c>
-      <c r="C65" t="s">
+      <c r="B67" t="s">
+        <v>221</v>
+      </c>
+      <c r="C67" t="s">
         <v>227</v>
       </c>
-      <c r="D65" t="s">
+      <c r="D67" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
+      <c r="B68" t="s">
         <v>229</v>
       </c>
-      <c r="B66" t="s">
-        <v>226</v>
-      </c>
-      <c r="C66" t="s">
+      <c r="C68" t="s">
         <v>230</v>
       </c>
-      <c r="D66" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
+      <c r="D68" t="s">
         <v>231</v>
       </c>
-      <c r="B67" t="s">
-        <v>226</v>
-      </c>
-      <c r="C67" t="s">
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
         <v>232</v>
       </c>
-      <c r="D67" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
+      <c r="B69" t="s">
+        <v>229</v>
+      </c>
+      <c r="C69" t="s">
         <v>233</v>
       </c>
-      <c r="B68" t="s">
+      <c r="D69" t="s">
         <v>234</v>
       </c>
-      <c r="C68" t="s">
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
         <v>235</v>
       </c>
-      <c r="D68" t="s">
+      <c r="B70" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
+      <c r="C70" t="s">
         <v>237</v>
       </c>
-      <c r="B69" t="s">
-        <v>234</v>
-      </c>
-      <c r="C69" t="s">
+      <c r="D70" t="s">
         <v>238</v>
       </c>
-      <c r="D69" t="s">
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
+      <c r="B71" t="s">
         <v>240</v>
       </c>
-      <c r="B70" t="s">
+      <c r="C71" t="s">
         <v>241</v>
       </c>
-      <c r="C70" t="s">
+      <c r="D71" t="s">
         <v>242</v>
       </c>
-      <c r="D70" t="s">
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="71" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
+      <c r="B72" t="s">
         <v>244</v>
       </c>
-      <c r="B71" t="s">
+      <c r="C72" t="s">
         <v>245</v>
       </c>
-      <c r="C71" t="s">
+      <c r="D72" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
         <v>246</v>
       </c>
-      <c r="D71" t="s">
+      <c r="B73" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="72" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
+      <c r="C73" t="s">
         <v>248</v>
       </c>
-      <c r="B72" t="s">
+      <c r="D73" t="s">
         <v>249</v>
       </c>
-      <c r="C72" t="s">
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
         <v>250</v>
       </c>
-      <c r="D72" t="s">
+      <c r="B74" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="73" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
+      <c r="C74" t="s">
         <v>252</v>
       </c>
-      <c r="B73" t="s">
+      <c r="D74" t="s">
         <v>253</v>
       </c>
-      <c r="C73" t="s">
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
         <v>254</v>
       </c>
-      <c r="D73" t="s">
+      <c r="B75" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="74" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
+      <c r="C75" t="s">
         <v>256</v>
       </c>
-      <c r="B74" t="s">
+      <c r="D75" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
         <v>257</v>
       </c>
-      <c r="C74" t="s">
+      <c r="B76" t="s">
         <v>258</v>
       </c>
-      <c r="D74" t="s">
+      <c r="C76" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="75" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
+      <c r="D76" t="s">
         <v>260</v>
       </c>
-      <c r="B75" t="s">
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
         <v>261</v>
       </c>
-      <c r="C75" t="s">
+      <c r="B77" t="s">
         <v>262</v>
       </c>
-      <c r="D75" t="s">
+      <c r="C77" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="76" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
+      <c r="D77" t="s">
         <v>264</v>
       </c>
-      <c r="B76" t="s">
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
         <v>265</v>
       </c>
-      <c r="C76" t="s">
+      <c r="B78" t="s">
         <v>266</v>
       </c>
-      <c r="D76" t="s">
+      <c r="C78" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="77" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
+      <c r="D78" t="s">
         <v>268</v>
       </c>
-      <c r="B77" t="s">
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
         <v>269</v>
       </c>
-      <c r="C77" t="s">
+      <c r="B79" t="s">
         <v>270</v>
       </c>
-      <c r="D77" t="s">
+      <c r="C79" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="78" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
+      <c r="D79" t="s">
         <v>272</v>
       </c>
-      <c r="B78" t="s">
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
         <v>273</v>
       </c>
-      <c r="C78" t="s">
+      <c r="B80" t="s">
         <v>274</v>
       </c>
-      <c r="D78" t="s">
+      <c r="C80" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="79" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
+      <c r="D80" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
         <v>276</v>
       </c>
-      <c r="B79" t="s">
+      <c r="B81" t="s">
+        <v>274</v>
+      </c>
+      <c r="C81" t="s">
         <v>277</v>
       </c>
-      <c r="C79" t="s">
+      <c r="D81" t="s">
         <v>278</v>
       </c>
-      <c r="D79" t="s">
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="80" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
+      <c r="B82" t="s">
         <v>280</v>
       </c>
-      <c r="B80" t="s">
+      <c r="C82" t="s">
         <v>281</v>
       </c>
-      <c r="C80" t="s">
+      <c r="D82" t="s">
         <v>282</v>
       </c>
-      <c r="D80" t="s">
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
         <v>283</v>
       </c>
-    </row>
-    <row r="81" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
+      <c r="B83" t="s">
         <v>284</v>
       </c>
-      <c r="B81" t="s">
-        <v>281</v>
-      </c>
-      <c r="C81" t="s">
+      <c r="C83" t="s">
         <v>285</v>
       </c>
-      <c r="D81" t="s">
+      <c r="D83" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="82" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
         <v>287</v>
       </c>
-      <c r="B82" t="s">
+      <c r="B84" t="s">
         <v>288</v>
       </c>
-      <c r="C82" t="s">
+      <c r="C84" t="s">
         <v>289</v>
       </c>
-      <c r="D82" t="s">
+      <c r="D84" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="83" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
         <v>291</v>
       </c>
-      <c r="B83" t="s">
+      <c r="B85" t="s">
         <v>292</v>
       </c>
-      <c r="C83" t="s">
+      <c r="C85" t="s">
         <v>293</v>
       </c>
-      <c r="D83" t="s">
+      <c r="D85" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="84" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
+      <c r="B86" t="s">
         <v>295</v>
       </c>
-      <c r="B84" t="s">
+      <c r="C86" t="s">
         <v>296</v>
       </c>
-      <c r="C84" t="s">
+      <c r="D86" t="s">
         <v>297</v>
       </c>
-      <c r="D84" t="s">
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="85" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
+      <c r="B87" t="s">
         <v>299</v>
       </c>
-      <c r="B85" t="s">
+      <c r="C87" t="s">
         <v>300</v>
       </c>
-      <c r="C85" t="s">
+      <c r="D87" t="s">
         <v>301</v>
       </c>
-      <c r="D85" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
         <v>302</v>
       </c>
-      <c r="B86" t="s">
+      <c r="B88" t="s">
         <v>303</v>
       </c>
-      <c r="C86" t="s">
+      <c r="C88" t="s">
         <v>304</v>
       </c>
-      <c r="D86" t="s">
+      <c r="D88" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="87" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
         <v>306</v>
       </c>
-      <c r="B87" t="s">
+      <c r="B89" t="s">
         <v>307</v>
       </c>
-      <c r="C87" t="s">
+      <c r="C89" t="s">
         <v>308</v>
       </c>
-      <c r="D87" t="s">
+      <c r="D89" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="88" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
         <v>310</v>
       </c>
-      <c r="B88" t="s">
+      <c r="B90" t="s">
         <v>311</v>
       </c>
-      <c r="C88" t="s">
+      <c r="C90" t="s">
         <v>312</v>
       </c>
-      <c r="D88" t="s">
+      <c r="D90" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="89" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
         <v>314</v>
       </c>
-      <c r="B89" t="s">
+      <c r="B91" t="s">
         <v>315</v>
       </c>
-      <c r="C89" t="s">
+      <c r="C91" t="s">
         <v>316</v>
       </c>
-      <c r="D89" t="s">
+      <c r="D91" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="90" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
         <v>318</v>
       </c>
-      <c r="B90" t="s">
+      <c r="B92" t="s">
         <v>319</v>
       </c>
-      <c r="C90" t="s">
+      <c r="C92" t="s">
         <v>320</v>
       </c>
-      <c r="D90" t="s">
+      <c r="D92" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="91" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
         <v>322</v>
       </c>
-      <c r="B91" t="s">
+      <c r="B93" t="s">
         <v>323</v>
       </c>
-      <c r="C91" t="s">
+      <c r="C93" t="s">
         <v>324</v>
       </c>
-      <c r="D91" t="s">
+      <c r="D93" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="92" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
         <v>326</v>
       </c>
-      <c r="B92" t="s">
+      <c r="B94" t="s">
         <v>327</v>
       </c>
-      <c r="C92" t="s">
+      <c r="C94" t="s">
         <v>328</v>
       </c>
-      <c r="D92" t="s">
+      <c r="D94" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="93" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A93" t="s">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
         <v>330</v>
       </c>
-      <c r="B93" t="s">
+      <c r="B95" t="s">
         <v>331</v>
       </c>
-      <c r="C93" t="s">
+      <c r="C95" t="s">
         <v>332</v>
       </c>
-      <c r="D93" t="s">
+      <c r="D95" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="94" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
         <v>334</v>
       </c>
-      <c r="B94" t="s">
+      <c r="B96" t="s">
         <v>335</v>
       </c>
-      <c r="C94" t="s">
+      <c r="C96" t="s">
         <v>336</v>
       </c>
-      <c r="D94" t="s">
+      <c r="D96" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="95" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
         <v>338</v>
       </c>
-      <c r="B95" t="s">
+      <c r="B97" t="s">
         <v>339</v>
       </c>
-      <c r="C95" t="s">
+      <c r="C97" t="s">
         <v>340</v>
       </c>
-      <c r="D95" t="s">
+      <c r="D97" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="96" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A96" t="s">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
         <v>342</v>
       </c>
-      <c r="B96" t="s">
+      <c r="B98" t="s">
         <v>343</v>
       </c>
-      <c r="C96" t="s">
+      <c r="C98" t="s">
         <v>344</v>
       </c>
-      <c r="D96" t="s">
+      <c r="D98" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="97" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A97" t="s">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
         <v>346</v>
       </c>
-      <c r="B97" t="s">
+      <c r="B99" t="s">
         <v>347</v>
       </c>
-      <c r="C97" t="s">
+      <c r="C99" t="s">
         <v>348</v>
       </c>
-      <c r="D97" t="s">
+      <c r="D99" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
         <v>349</v>
       </c>
-    </row>
-    <row r="98" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A98" t="s">
+      <c r="B100" t="s">
         <v>350</v>
       </c>
-      <c r="B98" t="s">
+      <c r="C100" t="s">
         <v>351</v>
       </c>
-      <c r="C98" t="s">
+      <c r="D100" t="s">
         <v>352</v>
       </c>
-      <c r="D98" t="s">
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
         <v>353</v>
       </c>
-    </row>
-    <row r="99" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A99" t="s">
+      <c r="B101" t="s">
         <v>354</v>
       </c>
-      <c r="B99" t="s">
+      <c r="C101" t="s">
         <v>355</v>
       </c>
-      <c r="C99" t="s">
+      <c r="D101" t="s">
         <v>356</v>
       </c>
-      <c r="D99" t="s">
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A102" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="100" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A100" t="s">
+      <c r="B102" t="s">
         <v>358</v>
       </c>
-      <c r="B100" t="s">
+      <c r="C102" t="s">
         <v>359</v>
       </c>
-      <c r="C100" t="s">
+      <c r="D102" t="s">
         <v>360</v>
       </c>
-      <c r="D100" t="s">
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A103" t="s">
         <v>361</v>
       </c>
-    </row>
-    <row r="101" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A101" t="s">
+      <c r="B103" t="s">
         <v>362</v>
       </c>
-      <c r="B101" t="s">
+      <c r="C103" t="s">
         <v>363</v>
       </c>
-      <c r="C101" t="s">
+      <c r="D103" t="s">
         <v>364</v>
       </c>
-      <c r="D101" t="s">
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
         <v>365</v>
       </c>
-    </row>
-    <row r="102" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A102" t="s">
+      <c r="B104" t="s">
         <v>366</v>
       </c>
-      <c r="B102" t="s">
+      <c r="C104" t="s">
         <v>367</v>
       </c>
-      <c r="C102" t="s">
+      <c r="D104" t="s">
         <v>368</v>
       </c>
-      <c r="D102" t="s">
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A105" t="s">
         <v>369</v>
       </c>
-    </row>
-    <row r="103" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A103" t="s">
+      <c r="B105" t="s">
         <v>370</v>
       </c>
-      <c r="B103" t="s">
+      <c r="C105" t="s">
         <v>371</v>
       </c>
-      <c r="C103" t="s">
+      <c r="D105" t="s">
         <v>372</v>
       </c>
-      <c r="D103" t="s">
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A106" t="s">
         <v>373</v>
       </c>
-    </row>
-    <row r="104" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A104" t="s">
+      <c r="B106" t="s">
         <v>374</v>
       </c>
-      <c r="B104" t="s">
+      <c r="C106" t="s">
         <v>375</v>
       </c>
-      <c r="C104" t="s">
+      <c r="D106" t="s">
         <v>376</v>
       </c>
-      <c r="D104" t="s">
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A107" t="s">
         <v>377</v>
       </c>
-    </row>
-    <row r="105" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A105" t="s">
+      <c r="B107" t="s">
         <v>378</v>
       </c>
-      <c r="B105" t="s">
+      <c r="C107" t="s">
         <v>379</v>
       </c>
-      <c r="C105" t="s">
+      <c r="D107" t="s">
         <v>380</v>
       </c>
-      <c r="D105" t="s">
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A108" t="s">
         <v>381</v>
       </c>
-    </row>
-    <row r="106" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A106" t="s">
+      <c r="B108" t="s">
         <v>382</v>
       </c>
-      <c r="B106" t="s">
+      <c r="C108" t="s">
         <v>383</v>
       </c>
-      <c r="C106" t="s">
+      <c r="D108" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A109" t="s">
         <v>384</v>
       </c>
-      <c r="D106" t="s">
+      <c r="B109" t="s">
         <v>385</v>
       </c>
-    </row>
-    <row r="107" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A107" t="s">
+      <c r="C109" t="s">
         <v>386</v>
       </c>
-      <c r="B107" t="s">
+      <c r="D109" t="s">
         <v>387</v>
       </c>
-      <c r="C107" t="s">
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A110" t="s">
         <v>388</v>
       </c>
-      <c r="D107" t="s">
+      <c r="B110" t="s">
         <v>389</v>
       </c>
-    </row>
-    <row r="108" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A108" t="s">
+      <c r="C110" t="s">
         <v>390</v>
       </c>
-      <c r="B108" t="s">
+      <c r="D110" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A111" t="s">
         <v>391</v>
       </c>
-      <c r="C108" t="s">
+      <c r="B111" t="s">
+        <v>389</v>
+      </c>
+      <c r="C111" t="s">
+        <v>390</v>
+      </c>
+      <c r="D111" t="s">
         <v>392</v>
       </c>
-      <c r="D108" t="s">
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A112" t="s">
         <v>393</v>
       </c>
-    </row>
-    <row r="109" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A109" t="s">
+      <c r="B112" t="s">
         <v>394</v>
       </c>
-      <c r="B109" t="s">
+      <c r="C112" t="s">
         <v>395</v>
       </c>
-      <c r="C109" t="s">
+      <c r="D112" t="s">
         <v>396</v>
       </c>
-      <c r="D109" t="s">
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A113" t="s">
         <v>397</v>
       </c>
-    </row>
-    <row r="110" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A110" t="s">
+      <c r="B113" t="s">
+        <v>394</v>
+      </c>
+      <c r="C113" t="s">
         <v>398</v>
       </c>
-      <c r="B110" t="s">
+      <c r="D113" t="s">
         <v>399</v>
       </c>
-      <c r="C110" t="s">
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A114" t="s">
         <v>400</v>
       </c>
-      <c r="D110" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="111" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A111" t="s">
+      <c r="B114" t="s">
         <v>401</v>
       </c>
-      <c r="B111" t="s">
-        <v>399</v>
-      </c>
-      <c r="C111" t="s">
-        <v>400</v>
-      </c>
-      <c r="D111" t="s">
+      <c r="C114" t="s">
         <v>402</v>
       </c>
-    </row>
-    <row r="112" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A112" t="s">
+      <c r="D114" t="s">
         <v>403</v>
       </c>
-      <c r="B112" t="s">
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A115" t="s">
         <v>404</v>
       </c>
-      <c r="C112" t="s">
+      <c r="B115" t="s">
         <v>405</v>
       </c>
-      <c r="D112" t="s">
+      <c r="C115" t="s">
+        <v>99</v>
+      </c>
+      <c r="D115" t="s">
         <v>406</v>
       </c>
     </row>
-    <row r="113" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A113" t="s">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A116" t="s">
         <v>407</v>
       </c>
-      <c r="B113" t="s">
-        <v>404</v>
-      </c>
-      <c r="C113" t="s">
+      <c r="B116" t="s">
         <v>408</v>
       </c>
-      <c r="D113" t="s">
+      <c r="C116" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="114" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A114" t="s">
+      <c r="D116" t="s">
         <v>410</v>
       </c>
-      <c r="B114" t="s">
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A117" t="s">
         <v>411</v>
       </c>
-      <c r="C114" t="s">
+      <c r="B117" t="s">
         <v>412</v>
       </c>
-      <c r="D114" t="s">
+      <c r="C117" t="s">
         <v>413</v>
       </c>
-    </row>
-    <row r="115" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A115" t="s">
+      <c r="D117" t="s">
         <v>414</v>
       </c>
-      <c r="B115" t="s">
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A118" t="s">
         <v>415</v>
       </c>
-      <c r="C115" t="s">
-        <v>102</v>
-      </c>
-      <c r="D115" t="s">
+      <c r="B118" t="s">
         <v>416</v>
       </c>
-    </row>
-    <row r="116" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A116" t="s">
+      <c r="C118" t="s">
         <v>417</v>
       </c>
-      <c r="B116" t="s">
+      <c r="D118" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A119" t="s">
         <v>418</v>
       </c>
-      <c r="C116" t="s">
+      <c r="B119" t="s">
+        <v>416</v>
+      </c>
+      <c r="C119" t="s">
         <v>419</v>
       </c>
-      <c r="D116" t="s">
+      <c r="D119" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A120" t="s">
         <v>420</v>
       </c>
-    </row>
-    <row r="117" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A117" t="s">
+      <c r="B120" t="s">
+        <v>416</v>
+      </c>
+      <c r="C120" t="s">
         <v>421</v>
       </c>
-      <c r="B117" t="s">
+      <c r="D120" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A121" t="s">
         <v>422</v>
       </c>
-      <c r="C117" t="s">
+      <c r="B121" t="s">
+        <v>416</v>
+      </c>
+      <c r="C121" t="s">
         <v>423</v>
       </c>
-      <c r="D117" t="s">
+      <c r="D121" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A122" t="s">
         <v>424</v>
       </c>
-    </row>
-    <row r="118" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A118" t="s">
+      <c r="B122" t="s">
         <v>425</v>
       </c>
-      <c r="B118" t="s">
+      <c r="C122" t="s">
         <v>426</v>
       </c>
-      <c r="C118" t="s">
+      <c r="D122" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A123" t="s">
         <v>427</v>
       </c>
-      <c r="D118" t="s">
+      <c r="B123" t="s">
         <v>428</v>
       </c>
-    </row>
-    <row r="119" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A119" t="s">
+      <c r="C123" t="s">
         <v>429</v>
       </c>
-      <c r="B119" t="s">
-        <v>426</v>
-      </c>
-      <c r="C119" t="s">
+      <c r="D123" t="s">
         <v>430</v>
       </c>
-      <c r="D119" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="120" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A120" t="s">
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A124" t="s">
         <v>431</v>
       </c>
-      <c r="B120" t="s">
-        <v>426</v>
-      </c>
-      <c r="C120" t="s">
+      <c r="B124" t="s">
         <v>432</v>
       </c>
-      <c r="D120" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="121" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A121" t="s">
+      <c r="C124" t="s">
         <v>433</v>
       </c>
-      <c r="B121" t="s">
-        <v>426</v>
-      </c>
-      <c r="C121" t="s">
+      <c r="D124" t="s">
         <v>434</v>
       </c>
-      <c r="D121" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="122" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A122" t="s">
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A125" t="s">
         <v>435</v>
       </c>
-      <c r="B122" t="s">
+      <c r="B125" t="s">
         <v>436</v>
       </c>
-      <c r="C122" t="s">
+      <c r="C125" t="s">
         <v>437</v>
       </c>
-      <c r="D122" t="s">
+      <c r="D125" t="s">
         <v>438</v>
       </c>
     </row>
-    <row r="123" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A123" t="s">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A126" t="s">
         <v>439</v>
       </c>
-      <c r="B123" t="s">
+      <c r="B126" t="s">
         <v>440</v>
       </c>
-      <c r="C123" t="s">
+      <c r="C126" t="s">
         <v>441</v>
       </c>
-      <c r="D123" t="s">
+      <c r="D126" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A127" t="s">
         <v>442</v>
       </c>
-    </row>
-    <row r="124" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A124" t="s">
+      <c r="B127" t="s">
         <v>443</v>
       </c>
-      <c r="B124" t="s">
+      <c r="C127" t="s">
         <v>444</v>
       </c>
-      <c r="C124" t="s">
+      <c r="D127" t="s">
         <v>445</v>
       </c>
-      <c r="D124" t="s">
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A128" t="s">
         <v>446</v>
       </c>
-    </row>
-    <row r="125" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A125" t="s">
+      <c r="B128" t="s">
         <v>447</v>
       </c>
-      <c r="B125" t="s">
+      <c r="C128" t="s">
         <v>448</v>
       </c>
-      <c r="C125" t="s">
+      <c r="D128" t="s">
         <v>449</v>
       </c>
-      <c r="D125" t="s">
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A129" t="s">
         <v>450</v>
       </c>
-    </row>
-    <row r="126" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A126" t="s">
+      <c r="B129" t="s">
         <v>451</v>
       </c>
-      <c r="B126" t="s">
+      <c r="C129" t="s">
         <v>452</v>
       </c>
-      <c r="C126" t="s">
+      <c r="D129" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A130" t="s">
         <v>453</v>
       </c>
-      <c r="D126" t="s">
+      <c r="B130" t="s">
         <v>454</v>
       </c>
-    </row>
-    <row r="127" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A127" t="s">
+      <c r="C130" t="s">
         <v>455</v>
       </c>
-      <c r="B127" t="s">
+      <c r="D130" t="s">
         <v>456</v>
       </c>
-      <c r="C127" t="s">
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A131" t="s">
         <v>457</v>
       </c>
-      <c r="D127" t="s">
+      <c r="B131" t="s">
+        <v>454</v>
+      </c>
+      <c r="C131" t="s">
         <v>458</v>
       </c>
-    </row>
-    <row r="128" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A128" t="s">
+      <c r="D131" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A132" t="s">
         <v>459</v>
       </c>
-      <c r="B128" t="s">
+      <c r="B132" t="s">
         <v>460</v>
       </c>
-      <c r="C128" t="s">
+      <c r="C132" t="s">
         <v>461</v>
       </c>
-      <c r="D128" t="s">
+      <c r="D132" t="s">
         <v>462</v>
       </c>
     </row>
-    <row r="129" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A129" t="s">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A133" t="s">
         <v>463</v>
       </c>
-      <c r="B129" t="s">
+      <c r="B133" t="s">
         <v>464</v>
       </c>
-      <c r="C129" t="s">
+      <c r="C133" t="s">
         <v>465</v>
       </c>
-      <c r="D129" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="130" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A130" t="s">
+      <c r="D133" t="s">
         <v>466</v>
       </c>
-      <c r="B130" t="s">
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A134" t="s">
         <v>467</v>
       </c>
-      <c r="C130" t="s">
+      <c r="B134" t="s">
+        <v>464</v>
+      </c>
+      <c r="C134" t="s">
         <v>468</v>
       </c>
-      <c r="D130" t="s">
+      <c r="D134" t="s">
         <v>469</v>
       </c>
     </row>
-    <row r="131" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A131" t="s">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A135" t="s">
         <v>470</v>
       </c>
-      <c r="B131" t="s">
-        <v>467</v>
-      </c>
-      <c r="C131" t="s">
+      <c r="B135" t="s">
         <v>471</v>
-      </c>
-      <c r="D131" t="s">
-        <v>469</v>
-      </c>
-    </row>
-    <row r="132" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A132" t="s">
-        <v>472</v>
-      </c>
-      <c r="B132" t="s">
-        <v>473</v>
-      </c>
-      <c r="C132" t="s">
-        <v>474</v>
-      </c>
-      <c r="D132" t="s">
-        <v>475</v>
-      </c>
-    </row>
-    <row r="133" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A133" t="s">
-        <v>476</v>
-      </c>
-      <c r="B133" t="s">
-        <v>477</v>
-      </c>
-      <c r="C133" t="s">
-        <v>478</v>
-      </c>
-      <c r="D133" t="s">
-        <v>479</v>
-      </c>
-    </row>
-    <row r="134" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A134" t="s">
-        <v>480</v>
-      </c>
-      <c r="B134" t="s">
-        <v>477</v>
-      </c>
-      <c r="C134" t="s">
-        <v>481</v>
-      </c>
-      <c r="D134" t="s">
-        <v>482</v>
-      </c>
-    </row>
-    <row r="135" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A135" t="s">
-        <v>483</v>
-      </c>
-      <c r="B135" t="s">
-        <v>484</v>
       </c>
       <c r="C135" t="s">
         <v>10</v>
       </c>
       <c r="D135" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="136" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
+        <v>472</v>
+      </c>
+      <c r="B136" t="s">
+        <v>473</v>
+      </c>
+      <c r="C136" t="s">
+        <v>474</v>
+      </c>
+      <c r="D136" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A137" t="s">
+        <v>476</v>
+      </c>
+      <c r="B137" t="s">
+        <v>477</v>
+      </c>
+      <c r="C137" t="s">
+        <v>478</v>
+      </c>
+      <c r="D137" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A138" t="s">
+        <v>480</v>
+      </c>
+      <c r="B138" t="s">
+        <v>481</v>
+      </c>
+      <c r="C138" t="s">
+        <v>482</v>
+      </c>
+      <c r="D138" t="s">
         <v>485</v>
       </c>
-      <c r="B136" t="s">
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A139" t="s">
+        <v>483</v>
+      </c>
+      <c r="B139" t="s">
+        <v>481</v>
+      </c>
+      <c r="C139" t="s">
+        <v>484</v>
+      </c>
+      <c r="D139" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A140" t="s">
         <v>486</v>
       </c>
-      <c r="C136" t="s">
+      <c r="B140" t="s">
         <v>487</v>
       </c>
-      <c r="D136" t="s">
+      <c r="C140" t="s">
         <v>488</v>
       </c>
-    </row>
-    <row r="137" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A137" t="s">
+      <c r="D140" t="s">
         <v>489</v>
       </c>
-      <c r="B137" t="s">
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A141" t="s">
         <v>490</v>
       </c>
-      <c r="C137" t="s">
+      <c r="B141" t="s">
         <v>491</v>
       </c>
-      <c r="D137" t="s">
+      <c r="C141" t="s">
         <v>492</v>
       </c>
-    </row>
-    <row r="138" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A138" t="s">
+      <c r="D141" t="s">
         <v>493</v>
       </c>
-      <c r="B138" t="s">
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A142" t="s">
         <v>494</v>
       </c>
-      <c r="C138" t="s">
+      <c r="B142" t="s">
         <v>495</v>
       </c>
-      <c r="D138" t="s">
+      <c r="C142" t="s">
         <v>496</v>
       </c>
-    </row>
-    <row r="139" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A139" t="s">
+      <c r="D142" t="s">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A143" t="s">
         <v>497</v>
       </c>
-      <c r="B139" t="s">
-        <v>494</v>
-      </c>
-      <c r="C139" t="s">
+      <c r="B143" t="s">
         <v>498</v>
       </c>
-      <c r="D139" t="s">
+      <c r="C143" t="s">
         <v>499</v>
       </c>
-    </row>
-    <row r="140" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A140" t="s">
+      <c r="D143" t="s">
         <v>500</v>
       </c>
-      <c r="B140" t="s">
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A144" t="s">
         <v>501</v>
       </c>
-      <c r="C140" t="s">
+      <c r="B144" t="s">
         <v>502</v>
       </c>
-      <c r="D140" t="s">
+      <c r="C144" t="s">
         <v>503</v>
       </c>
-    </row>
-    <row r="141" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A141" t="s">
+      <c r="D144" t="s">
         <v>504</v>
       </c>
-      <c r="B141" t="s">
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A145" t="s">
         <v>505</v>
       </c>
-      <c r="C141" t="s">
+      <c r="B145" t="s">
         <v>506</v>
-      </c>
-      <c r="D141" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="142" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A142" t="s">
-        <v>508</v>
-      </c>
-      <c r="B142" t="s">
-        <v>509</v>
-      </c>
-      <c r="C142" t="s">
-        <v>510</v>
-      </c>
-      <c r="D142" t="s">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="143" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A143" t="s">
-        <v>512</v>
-      </c>
-      <c r="B143" t="s">
-        <v>513</v>
-      </c>
-      <c r="C143" t="s">
-        <v>514</v>
-      </c>
-      <c r="D143" t="s">
-        <v>515</v>
-      </c>
-    </row>
-    <row r="144" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A144" t="s">
-        <v>516</v>
-      </c>
-      <c r="B144" t="s">
-        <v>517</v>
-      </c>
-      <c r="C144" t="s">
-        <v>518</v>
-      </c>
-      <c r="D144" t="s">
-        <v>519</v>
-      </c>
-    </row>
-    <row r="145" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A145" t="s">
-        <v>520</v>
-      </c>
-      <c r="B145" t="s">
-        <v>521</v>
       </c>
       <c r="C145" t="s">
         <v>10</v>
       </c>
       <c r="D145" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="146" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
+        <v>507</v>
+      </c>
+      <c r="B146" t="s">
+        <v>508</v>
+      </c>
+      <c r="C146" t="s">
+        <v>509</v>
+      </c>
+      <c r="D146" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A147" t="s">
+        <v>511</v>
+      </c>
+      <c r="B147" t="s">
+        <v>512</v>
+      </c>
+      <c r="C147" t="s">
+        <v>513</v>
+      </c>
+      <c r="D147" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A148" t="s">
+        <v>514</v>
+      </c>
+      <c r="B148" t="s">
+        <v>515</v>
+      </c>
+      <c r="C148" t="s">
+        <v>516</v>
+      </c>
+      <c r="D148" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A149" t="s">
+        <v>518</v>
+      </c>
+      <c r="B149" t="s">
+        <v>519</v>
+      </c>
+      <c r="C149" t="s">
+        <v>520</v>
+      </c>
+      <c r="D149" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A150" t="s">
         <v>522</v>
       </c>
-      <c r="B146" t="s">
+      <c r="B150" t="s">
         <v>523</v>
       </c>
-      <c r="C146" t="s">
+      <c r="C150" t="s">
         <v>524</v>
       </c>
-      <c r="D146" t="s">
+      <c r="D150" t="s">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A151" t="s">
         <v>525</v>
       </c>
-    </row>
-    <row r="147" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A147" t="s">
+      <c r="B151" t="s">
         <v>526</v>
       </c>
-      <c r="B147" t="s">
+      <c r="C151" t="s">
         <v>527</v>
       </c>
-      <c r="C147" t="s">
+      <c r="D151" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A152" t="s">
         <v>528</v>
       </c>
-      <c r="D147" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="148" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A148" t="s">
+      <c r="B152" t="s">
         <v>529</v>
       </c>
-      <c r="B148" t="s">
+      <c r="C152" t="s">
         <v>530</v>
       </c>
-      <c r="C148" t="s">
+      <c r="D152" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A153" t="s">
         <v>531</v>
       </c>
-      <c r="D148" t="s">
+      <c r="B153" t="s">
         <v>532</v>
       </c>
-    </row>
-    <row r="149" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A149" t="s">
+      <c r="C153" t="s">
         <v>533</v>
       </c>
-      <c r="B149" t="s">
+      <c r="D153" t="s">
         <v>534</v>
       </c>
-      <c r="C149" t="s">
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A154" t="s">
         <v>535</v>
       </c>
-      <c r="D149" t="s">
+      <c r="B154" t="s">
         <v>536</v>
       </c>
-    </row>
-    <row r="150" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A150" t="s">
+      <c r="C154" t="s">
+        <v>101</v>
+      </c>
+      <c r="D154" t="s">
         <v>537</v>
       </c>
-      <c r="B150" t="s">
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A155" t="s">
         <v>538</v>
       </c>
-      <c r="C150" t="s">
+      <c r="B155" t="s">
         <v>539</v>
       </c>
-      <c r="D150" t="s">
+      <c r="C155" t="s">
         <v>540</v>
       </c>
-    </row>
-    <row r="151" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A151" t="s">
+      <c r="D155" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A156" t="s">
         <v>541</v>
       </c>
-      <c r="B151" t="s">
+      <c r="B156" t="s">
         <v>542</v>
       </c>
-      <c r="C151" t="s">
+      <c r="C156" t="s">
         <v>543</v>
       </c>
-      <c r="D151" t="s">
+      <c r="D156" t="s">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A157" t="s">
         <v>544</v>
       </c>
-    </row>
-    <row r="152" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A152" t="s">
+      <c r="B157" t="s">
         <v>545</v>
       </c>
-      <c r="B152" t="s">
+      <c r="C157" t="s">
         <v>546</v>
       </c>
-      <c r="C152" t="s">
+      <c r="D157" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A158" t="s">
         <v>547</v>
       </c>
-      <c r="D152" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="153" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A153" t="s">
+      <c r="B158" t="s">
         <v>548</v>
       </c>
-      <c r="B153" t="s">
+      <c r="C158" t="s">
         <v>549</v>
       </c>
-      <c r="C153" t="s">
+      <c r="D158" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A159" t="s">
         <v>550</v>
       </c>
-      <c r="D153" t="s">
+      <c r="B159" t="s">
         <v>551</v>
-      </c>
-    </row>
-    <row r="154" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A154" t="s">
-        <v>552</v>
-      </c>
-      <c r="B154" t="s">
-        <v>553</v>
-      </c>
-      <c r="C154" t="s">
-        <v>104</v>
-      </c>
-      <c r="D154" t="s">
-        <v>554</v>
-      </c>
-    </row>
-    <row r="155" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A155" t="s">
-        <v>555</v>
-      </c>
-      <c r="B155" t="s">
-        <v>556</v>
-      </c>
-      <c r="C155" t="s">
-        <v>557</v>
-      </c>
-      <c r="D155" t="s">
-        <v>558</v>
-      </c>
-    </row>
-    <row r="156" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A156" t="s">
-        <v>559</v>
-      </c>
-      <c r="B156" t="s">
-        <v>560</v>
-      </c>
-      <c r="C156" t="s">
-        <v>561</v>
-      </c>
-      <c r="D156" t="s">
-        <v>562</v>
-      </c>
-    </row>
-    <row r="157" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A157" t="s">
-        <v>563</v>
-      </c>
-      <c r="B157" t="s">
-        <v>564</v>
-      </c>
-      <c r="C157" t="s">
-        <v>565</v>
-      </c>
-      <c r="D157" t="s">
-        <v>566</v>
-      </c>
-    </row>
-    <row r="158" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A158" t="s">
-        <v>567</v>
-      </c>
-      <c r="B158" t="s">
-        <v>568</v>
-      </c>
-      <c r="C158" t="s">
-        <v>569</v>
-      </c>
-      <c r="D158" t="s">
-        <v>570</v>
-      </c>
-    </row>
-    <row r="159" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A159" t="s">
-        <v>571</v>
-      </c>
-      <c r="B159" t="s">
-        <v>572</v>
       </c>
       <c r="C159" t="s">
         <v>10</v>
       </c>
       <c r="D159" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="160" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
+        <v>552</v>
+      </c>
+      <c r="B160" t="s">
+        <v>553</v>
+      </c>
+      <c r="C160" t="s">
+        <v>554</v>
+      </c>
+      <c r="D160" t="s">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A161" t="s">
+        <v>555</v>
+      </c>
+      <c r="B161" t="s">
+        <v>553</v>
+      </c>
+      <c r="C161" t="s">
+        <v>556</v>
+      </c>
+      <c r="D161" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A162" t="s">
+        <v>557</v>
+      </c>
+      <c r="B162" t="s">
+        <v>558</v>
+      </c>
+      <c r="C162" t="s">
+        <v>559</v>
+      </c>
+      <c r="D162" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A163" t="s">
+        <v>561</v>
+      </c>
+      <c r="B163" t="s">
+        <v>562</v>
+      </c>
+      <c r="C163" t="s">
+        <v>563</v>
+      </c>
+      <c r="D163" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A164" t="s">
+        <v>564</v>
+      </c>
+      <c r="B164" t="s">
+        <v>565</v>
+      </c>
+      <c r="C164" t="s">
+        <v>566</v>
+      </c>
+      <c r="D164" t="s">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A165" t="s">
+        <v>567</v>
+      </c>
+      <c r="B165" t="s">
+        <v>568</v>
+      </c>
+      <c r="C165" t="s">
+        <v>569</v>
+      </c>
+      <c r="D165" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A166" t="s">
+        <v>570</v>
+      </c>
+      <c r="B166" t="s">
+        <v>571</v>
+      </c>
+      <c r="C166" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A167" t="s">
         <v>573</v>
       </c>
-      <c r="B160" t="s">
+      <c r="B167" t="s">
         <v>574</v>
       </c>
-      <c r="C160" t="s">
+      <c r="C167" t="s">
         <v>575</v>
       </c>
-      <c r="D160" t="s">
+      <c r="D167" t="s">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A168" t="s">
         <v>576</v>
       </c>
-    </row>
-    <row r="161" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A161" t="s">
+      <c r="B168" t="s">
         <v>577</v>
       </c>
-      <c r="B161" t="s">
-        <v>574</v>
-      </c>
-      <c r="C161" t="s">
+      <c r="C168" t="s">
+        <v>99</v>
+      </c>
+      <c r="D168" t="s">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A169" t="s">
         <v>578</v>
       </c>
-      <c r="D161" t="s">
+      <c r="B169" t="s">
         <v>579</v>
       </c>
-    </row>
-    <row r="162" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A162" t="s">
+      <c r="C169" t="s">
         <v>580</v>
       </c>
-      <c r="B162" t="s">
+      <c r="D169" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A170" t="s">
         <v>581</v>
       </c>
-      <c r="C162" t="s">
+      <c r="B170" t="s">
         <v>582</v>
       </c>
-      <c r="D162" t="s">
+      <c r="C170" t="s">
         <v>583</v>
       </c>
-    </row>
-    <row r="163" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A163" t="s">
+      <c r="D170" t="s">
         <v>584</v>
       </c>
-      <c r="B163" t="s">
+    </row>
+    <row r="171" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A171" t="s">
         <v>585</v>
       </c>
-      <c r="C163" t="s">
+      <c r="B171" t="s">
         <v>586</v>
       </c>
-      <c r="D163" t="s">
+      <c r="C171" t="s">
         <v>587</v>
       </c>
-    </row>
-    <row r="164" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A164" t="s">
+      <c r="D171" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A172" t="s">
         <v>588</v>
       </c>
-      <c r="B164" t="s">
+      <c r="B172" t="s">
         <v>589</v>
       </c>
-      <c r="C164" t="s">
+      <c r="C172" t="s">
         <v>590</v>
       </c>
-      <c r="D164" t="s">
+      <c r="D172" t="s">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A173" t="s">
         <v>591</v>
       </c>
-    </row>
-    <row r="165" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A165" t="s">
+      <c r="B173" t="s">
         <v>592</v>
       </c>
-      <c r="B165" t="s">
+      <c r="C173" t="s">
         <v>593</v>
       </c>
-      <c r="C165" t="s">
+      <c r="D173" t="s">
         <v>594</v>
       </c>
-      <c r="D165" t="s">
+    </row>
+    <row r="174" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A174" t="s">
         <v>595</v>
       </c>
-    </row>
-    <row r="166" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A166" t="s">
+      <c r="B174" t="s">
         <v>596</v>
       </c>
-      <c r="B166" t="s">
+      <c r="C174" t="s">
         <v>597</v>
       </c>
-      <c r="C166" t="s">
+      <c r="D174" t="s">
         <v>598</v>
       </c>
-      <c r="D166" t="s">
+    </row>
+    <row r="175" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A175" t="s">
         <v>599</v>
       </c>
-    </row>
-    <row r="167" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A167" t="s">
+      <c r="B175" t="s">
         <v>600</v>
       </c>
-      <c r="B167" t="s">
+      <c r="C175" t="s">
         <v>601</v>
       </c>
-      <c r="C167" t="s">
+      <c r="D175" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A176" t="s">
         <v>602</v>
       </c>
-      <c r="D167" t="s">
+      <c r="B176" t="s">
+        <v>600</v>
+      </c>
+      <c r="C176" t="s">
         <v>603</v>
       </c>
-    </row>
-    <row r="168" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A168" t="s">
+      <c r="D176" t="s">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A177" t="s">
         <v>604</v>
       </c>
-      <c r="B168" t="s">
+      <c r="B177" t="s">
         <v>605</v>
       </c>
-      <c r="C168" t="s">
-        <v>102</v>
-      </c>
-      <c r="D168" t="s">
+      <c r="C177" t="s">
         <v>606</v>
       </c>
-    </row>
-    <row r="169" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A169" t="s">
+      <c r="D177" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A178" t="s">
         <v>607</v>
       </c>
-      <c r="B169" t="s">
+      <c r="B178" t="s">
         <v>608</v>
       </c>
-      <c r="C169" t="s">
+      <c r="C178" t="s">
         <v>609</v>
       </c>
-      <c r="D169" t="s">
+      <c r="D178" t="s">
         <v>610</v>
       </c>
     </row>
-    <row r="170" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A170" t="s">
+    <row r="179" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A179" t="s">
         <v>611</v>
       </c>
-      <c r="B170" t="s">
+      <c r="B179" t="s">
         <v>612</v>
       </c>
-      <c r="C170" t="s">
+      <c r="C179" t="s">
         <v>613</v>
       </c>
-      <c r="D170" t="s">
+      <c r="D179" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A180" t="s">
         <v>614</v>
       </c>
-    </row>
-    <row r="171" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A171" t="s">
+      <c r="B180" t="s">
         <v>615</v>
       </c>
-      <c r="B171" t="s">
+      <c r="C180" t="s">
         <v>616</v>
       </c>
-      <c r="C171" t="s">
+      <c r="D180" t="s">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A181" t="s">
         <v>617</v>
       </c>
-      <c r="D171" t="s">
+      <c r="B181" t="s">
+        <v>615</v>
+      </c>
+      <c r="C181" t="s">
         <v>618</v>
       </c>
-    </row>
-    <row r="172" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A172" t="s">
+      <c r="D181" t="s">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A182" t="s">
         <v>619</v>
       </c>
-      <c r="B172" t="s">
+      <c r="B182" t="s">
         <v>620</v>
       </c>
-      <c r="C172" t="s">
+      <c r="C182" t="s">
         <v>621</v>
       </c>
-      <c r="D172" t="s">
+      <c r="D182" t="s">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="183" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A183" t="s">
         <v>622</v>
       </c>
-    </row>
-    <row r="173" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A173" t="s">
+      <c r="B183" t="s">
         <v>623</v>
       </c>
-      <c r="B173" t="s">
+      <c r="C183" t="s">
         <v>624</v>
       </c>
-      <c r="C173" t="s">
+      <c r="D183" t="s">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A184" t="s">
         <v>625</v>
       </c>
-      <c r="D173" t="s">
+      <c r="B184" t="s">
         <v>626</v>
       </c>
-    </row>
-    <row r="174" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A174" t="s">
+      <c r="C184" t="s">
         <v>627</v>
       </c>
-      <c r="B174" t="s">
+      <c r="D184" t="s">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A185" t="s">
         <v>628</v>
       </c>
-      <c r="C174" t="s">
+      <c r="B185" t="s">
         <v>629</v>
       </c>
-      <c r="D174" t="s">
+      <c r="C185" t="s">
         <v>630</v>
       </c>
-    </row>
-    <row r="175" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A175" t="s">
+      <c r="D185" t="s">
         <v>631</v>
       </c>
-      <c r="B175" t="s">
+    </row>
+    <row r="186" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A186" t="s">
         <v>632</v>
       </c>
-      <c r="C175" t="s">
+      <c r="B186" t="s">
+        <v>629</v>
+      </c>
+      <c r="C186" t="s">
         <v>633</v>
       </c>
-      <c r="D175" t="s">
+      <c r="D186" t="s">
+        <v>676</v>
+      </c>
+    </row>
+    <row r="187" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A187" t="s">
         <v>634</v>
       </c>
-    </row>
-    <row r="176" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A176" t="s">
+      <c r="B187" t="s">
         <v>635</v>
       </c>
-      <c r="B176" t="s">
-        <v>632</v>
-      </c>
-      <c r="C176" t="s">
+      <c r="C187" t="s">
         <v>636</v>
-      </c>
-      <c r="D176" t="s">
-        <v>634</v>
-      </c>
-    </row>
-    <row r="177" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A177" t="s">
-        <v>637</v>
-      </c>
-      <c r="B177" t="s">
-        <v>638</v>
-      </c>
-      <c r="C177" t="s">
-        <v>639</v>
-      </c>
-      <c r="D177" t="s">
-        <v>640</v>
-      </c>
-    </row>
-    <row r="178" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A178" t="s">
-        <v>641</v>
-      </c>
-      <c r="B178" t="s">
-        <v>642</v>
-      </c>
-      <c r="C178" t="s">
-        <v>643</v>
-      </c>
-      <c r="D178" t="s">
-        <v>644</v>
-      </c>
-    </row>
-    <row r="179" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A179" t="s">
-        <v>645</v>
-      </c>
-      <c r="B179" t="s">
-        <v>646</v>
-      </c>
-      <c r="C179" t="s">
-        <v>647</v>
-      </c>
-      <c r="D179" t="s">
-        <v>648</v>
-      </c>
-    </row>
-    <row r="180" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A180" t="s">
-        <v>649</v>
-      </c>
-      <c r="B180" t="s">
-        <v>650</v>
-      </c>
-      <c r="C180" t="s">
-        <v>651</v>
-      </c>
-      <c r="D180" t="s">
-        <v>652</v>
-      </c>
-    </row>
-    <row r="181" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A181" t="s">
-        <v>653</v>
-      </c>
-      <c r="B181" t="s">
-        <v>650</v>
-      </c>
-      <c r="C181" t="s">
-        <v>654</v>
-      </c>
-      <c r="D181" t="s">
-        <v>652</v>
-      </c>
-    </row>
-    <row r="182" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A182" t="s">
-        <v>655</v>
-      </c>
-      <c r="B182" t="s">
-        <v>656</v>
-      </c>
-      <c r="C182" t="s">
-        <v>657</v>
-      </c>
-      <c r="D182" t="s">
-        <v>658</v>
-      </c>
-    </row>
-    <row r="183" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A183" t="s">
-        <v>659</v>
-      </c>
-      <c r="B183" t="s">
-        <v>660</v>
-      </c>
-      <c r="C183" t="s">
-        <v>661</v>
-      </c>
-      <c r="D183" t="s">
-        <v>662</v>
-      </c>
-    </row>
-    <row r="184" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A184" t="s">
-        <v>663</v>
-      </c>
-      <c r="B184" t="s">
-        <v>664</v>
-      </c>
-      <c r="C184" t="s">
-        <v>665</v>
-      </c>
-      <c r="D184" t="s">
-        <v>666</v>
-      </c>
-    </row>
-    <row r="185" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A185" t="s">
-        <v>667</v>
-      </c>
-      <c r="B185" t="s">
-        <v>668</v>
-      </c>
-      <c r="C185" t="s">
-        <v>669</v>
-      </c>
-      <c r="D185" t="s">
-        <v>670</v>
-      </c>
-    </row>
-    <row r="186" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A186" t="s">
-        <v>671</v>
-      </c>
-      <c r="B186" t="s">
-        <v>668</v>
-      </c>
-      <c r="C186" t="s">
-        <v>672</v>
-      </c>
-      <c r="D186" t="s">
-        <v>673</v>
-      </c>
-    </row>
-    <row r="187" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A187" t="s">
-        <v>674</v>
-      </c>
-      <c r="B187" t="s">
-        <v>675</v>
-      </c>
-      <c r="C187" t="s">
-        <v>676</v>
       </c>
       <c r="D187" t="s">
         <v>677</v>
       </c>
     </row>
-    <row r="188" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
+        <v>637</v>
+      </c>
+      <c r="B188" t="s">
+        <v>638</v>
+      </c>
+      <c r="C188" t="s">
+        <v>639</v>
+      </c>
+      <c r="D188" t="s">
         <v>678</v>
       </c>
-      <c r="B188" t="s">
+    </row>
+    <row r="189" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A189" t="s">
+        <v>640</v>
+      </c>
+      <c r="B189" t="s">
+        <v>641</v>
+      </c>
+      <c r="C189" t="s">
+        <v>642</v>
+      </c>
+      <c r="D189" t="s">
         <v>679</v>
       </c>
-      <c r="C188" t="s">
-        <v>680</v>
-      </c>
-      <c r="D188" t="s">
-        <v>681</v>
-      </c>
-    </row>
-    <row r="189" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A189" t="s">
-        <v>682</v>
-      </c>
-      <c r="B189" t="s">
-        <v>683</v>
-      </c>
-      <c r="C189" t="s">
-        <v>684</v>
-      </c>
-      <c r="D189" t="s">
-        <v>685</v>
-      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>